<commit_message>
Cambio de una letra en la control cx
</commit_message>
<xml_diff>
--- a/Control de cirugía 2022.xlsx
+++ b/Control de cirugía 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\control_cirugias_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4CD5CE-999E-43ED-A219-54616AAFEFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3F092C-3182-49DC-86C1-9D4BFF804032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2395,51 +2395,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2504,6 +2459,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2511,63 +2511,6 @@
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2685,6 +2628,63 @@
       </font>
       <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2862,17 +2862,17 @@
     <tableColumn id="2" xr3:uid="{A57A96DA-EF5A-46FB-AAF3-E965AB7FF857}" name="INSTITUCION" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{D99350EC-FC2D-48EE-930C-B9804507D8C0}" name="MEDICO" dataDxfId="10"/>
     <tableColumn id="4" xr3:uid="{A5F7129F-BCF1-4A07-9834-3B15950B9E74}" name="PACIENTE " dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{36FED70C-D839-4A77-A585-032A152AD588}" name="SISTEMAS" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{93E442AB-2AA6-4189-A00F-44A2C4C05E75}" name="PLACAS" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{38AC5BC3-48A5-47EC-BC8F-657A0E53640D}" name="MOTOR " dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{FABD216D-7570-48F2-8C2B-47466DF0C464}" name="FECHA DE ENTREGA " dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{173BE5C6-2216-4117-A6B4-35D9D571E087}" name="FECHA DE CIRUGIA " dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{AEDA8538-8FA1-411A-BDF7-45006F61BCA0}" name="FECHA DE RECOJO  " dataDxfId="6">
+    <tableColumn id="7" xr3:uid="{36FED70C-D839-4A77-A585-032A152AD588}" name="SISTEMAS" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{93E442AB-2AA6-4189-A00F-44A2C4C05E75}" name="PLACAS" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{38AC5BC3-48A5-47EC-BC8F-657A0E53640D}" name="MOTOR " dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{FABD216D-7570-48F2-8C2B-47466DF0C464}" name="FECHA DE ENTREGA " dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{173BE5C6-2216-4117-A6B4-35D9D571E087}" name="FECHA DE CIRUGIA " dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{AEDA8538-8FA1-411A-BDF7-45006F61BCA0}" name="FECHA DE RECOJO  " dataDxfId="3">
       <calculatedColumnFormula>I2+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{1260940A-73A2-4317-B965-A0F8AEE0B1AC}" name="CIRUGIA" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{866E3850-9961-4C6A-8463-32897B46C826}" name="IMPLANTE UTILIZADO (PLACA)" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{A3348460-1786-4179-B55F-AED445FE115F}" name="Columna1" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{1260940A-73A2-4317-B965-A0F8AEE0B1AC}" name="CIRUGIA" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{866E3850-9961-4C6A-8463-32897B46C826}" name="IMPLANTE UTILIZADO (PLACA)" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{A3348460-1786-4179-B55F-AED445FE115F}" name="Columna1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3146,8 +3146,8 @@
   </sheetPr>
   <dimension ref="A1:M200"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A163" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I172" sqref="I172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3156,8 +3156,8 @@
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" style="93" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" style="93" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" style="78" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="78" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" customWidth="1"/>
@@ -3182,10 +3182,10 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="83" t="s">
+      <c r="E1" s="68" t="s">
         <v>553</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="F1" s="68" t="s">
         <v>554</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -3223,10 +3223,10 @@
       <c r="D2" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="69" t="s">
         <v>457</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="69" t="s">
         <v>457</v>
       </c>
       <c r="G2" s="38" t="s">
@@ -3264,10 +3264,10 @@
       <c r="D3" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F3" s="85" t="s">
+      <c r="F3" s="70" t="s">
         <v>551</v>
       </c>
       <c r="G3" s="38" t="s">
@@ -3305,10 +3305,10 @@
       <c r="D4" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="85" t="s">
+      <c r="E4" s="70" t="s">
         <v>537</v>
       </c>
-      <c r="F4" s="85" t="s">
+      <c r="F4" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G4" s="38" t="s">
@@ -3346,10 +3346,10 @@
       <c r="D5" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="85" t="s">
+      <c r="E5" s="70" t="s">
         <v>457</v>
       </c>
-      <c r="F5" s="85" t="s">
+      <c r="F5" s="70" t="s">
         <v>457</v>
       </c>
       <c r="G5" s="38" t="s">
@@ -3387,10 +3387,10 @@
       <c r="D6" s="39" t="s">
         <v>299</v>
       </c>
-      <c r="E6" s="85" t="s">
+      <c r="E6" s="70" t="s">
         <v>555</v>
       </c>
-      <c r="F6" s="85" t="s">
+      <c r="F6" s="70" t="s">
         <v>555</v>
       </c>
       <c r="G6" s="38" t="s">
@@ -3428,10 +3428,10 @@
       <c r="D7" s="39" t="s">
         <v>301</v>
       </c>
-      <c r="E7" s="85" t="s">
+      <c r="E7" s="70" t="s">
         <v>556</v>
       </c>
-      <c r="F7" s="85" t="s">
+      <c r="F7" s="70" t="s">
         <v>556</v>
       </c>
       <c r="G7" s="38" t="s">
@@ -3469,10 +3469,10 @@
       <c r="D8" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="85" t="s">
+      <c r="E8" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F8" s="85" t="s">
+      <c r="F8" s="70" t="s">
         <v>557</v>
       </c>
       <c r="G8" s="38" t="s">
@@ -3510,10 +3510,10 @@
       <c r="D9" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="85" t="s">
+      <c r="E9" s="70" t="s">
         <v>561</v>
       </c>
-      <c r="F9" s="85" t="s">
+      <c r="F9" s="70" t="s">
         <v>561</v>
       </c>
       <c r="G9" s="38" t="s">
@@ -3551,10 +3551,10 @@
       <c r="D10" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="85" t="s">
+      <c r="E10" s="70" t="s">
         <v>537</v>
       </c>
-      <c r="F10" s="85" t="s">
+      <c r="F10" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G10" s="38" t="s">
@@ -3591,10 +3591,10 @@
       <c r="D11" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="86" t="s">
+      <c r="E11" s="71" t="s">
         <v>538</v>
       </c>
-      <c r="F11" s="86" t="s">
+      <c r="F11" s="71" t="s">
         <v>540</v>
       </c>
       <c r="G11" s="43" t="s">
@@ -3632,13 +3632,13 @@
       <c r="D12" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="85" t="s">
+      <c r="E12" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="85" t="s">
+      <c r="F12" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="80" t="s">
+      <c r="G12" s="65" t="s">
         <v>18</v>
       </c>
       <c r="H12" s="55">
@@ -3673,10 +3673,10 @@
       <c r="D13" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="E13" s="85" t="s">
+      <c r="E13" s="70" t="s">
         <v>562</v>
       </c>
-      <c r="F13" s="85" t="s">
+      <c r="F13" s="70" t="s">
         <v>558</v>
       </c>
       <c r="G13" s="38" t="s">
@@ -3714,10 +3714,10 @@
       <c r="D14" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="85" t="s">
+      <c r="E14" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F14" s="85" t="s">
+      <c r="F14" s="70" t="s">
         <v>542</v>
       </c>
       <c r="G14" s="38" t="s">
@@ -3755,10 +3755,10 @@
       <c r="D15" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="85" t="s">
+      <c r="E15" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F15" s="85" t="s">
+      <c r="F15" s="70" t="s">
         <v>546</v>
       </c>
       <c r="G15" s="38" t="s">
@@ -3796,10 +3796,10 @@
       <c r="D16" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="85" t="s">
+      <c r="E16" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F16" s="85" t="s">
+      <c r="F16" s="70" t="s">
         <v>540</v>
       </c>
       <c r="G16" s="38" t="s">
@@ -3836,10 +3836,10 @@
       <c r="D17" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="85" t="s">
+      <c r="E17" s="70" t="s">
         <v>457</v>
       </c>
-      <c r="F17" s="85" t="s">
+      <c r="F17" s="70" t="s">
         <v>457</v>
       </c>
       <c r="G17" s="38" t="s">
@@ -3877,10 +3877,10 @@
       <c r="D18" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="87" t="s">
+      <c r="E18" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="87" t="s">
+      <c r="F18" s="72" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="44" t="s">
@@ -3918,10 +3918,10 @@
       <c r="D19" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="85" t="s">
+      <c r="E19" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="85" t="s">
+      <c r="F19" s="70" t="s">
         <v>30</v>
       </c>
       <c r="G19" s="38" t="s">
@@ -3959,10 +3959,10 @@
       <c r="D20" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="85" t="s">
+      <c r="E20" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F20" s="85" t="s">
+      <c r="F20" s="70" t="s">
         <v>558</v>
       </c>
       <c r="G20" s="38" t="s">
@@ -4000,10 +4000,10 @@
       <c r="D21" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="85" t="s">
+      <c r="E21" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F21" s="85" t="s">
+      <c r="F21" s="70" t="s">
         <v>559</v>
       </c>
       <c r="G21" s="38" t="s">
@@ -4041,10 +4041,10 @@
       <c r="D22" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="85" t="s">
+      <c r="E22" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="85" t="s">
+      <c r="F22" s="70" t="s">
         <v>18</v>
       </c>
       <c r="G22" s="38" t="s">
@@ -4082,10 +4082,10 @@
       <c r="D23" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="85" t="s">
+      <c r="E23" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F23" s="85" t="s">
+      <c r="F23" s="70" t="s">
         <v>540</v>
       </c>
       <c r="G23" s="38" t="s">
@@ -4123,10 +4123,10 @@
       <c r="D24" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="E24" s="85" t="s">
+      <c r="E24" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F24" s="85" t="s">
+      <c r="F24" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G24" s="38" t="s">
@@ -4164,10 +4164,10 @@
       <c r="D25" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="E25" s="85" t="s">
+      <c r="E25" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F25" s="85" t="s">
+      <c r="F25" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G25" s="38" t="s">
@@ -4205,10 +4205,10 @@
       <c r="D26" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="E26" s="85" t="s">
+      <c r="E26" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F26" s="85" t="s">
+      <c r="F26" s="70" t="s">
         <v>540</v>
       </c>
       <c r="G26" s="38" t="s">
@@ -4246,10 +4246,10 @@
       <c r="D27" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="E27" s="88" t="s">
+      <c r="E27" s="73" t="s">
         <v>563</v>
       </c>
-      <c r="F27" s="88" t="s">
+      <c r="F27" s="73" t="s">
         <v>542</v>
       </c>
       <c r="G27" s="38" t="s">
@@ -4286,10 +4286,10 @@
       <c r="D28" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="E28" s="85" t="s">
+      <c r="E28" s="70" t="s">
         <v>564</v>
       </c>
-      <c r="F28" s="85" t="s">
+      <c r="F28" s="70" t="s">
         <v>564</v>
       </c>
       <c r="G28" s="38" t="s">
@@ -4326,10 +4326,10 @@
       <c r="D29" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="E29" s="85" t="s">
+      <c r="E29" s="70" t="s">
         <v>555</v>
       </c>
-      <c r="F29" s="85" t="s">
+      <c r="F29" s="70" t="s">
         <v>552</v>
       </c>
       <c r="G29" s="38" t="s">
@@ -4366,10 +4366,10 @@
       <c r="D30" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="E30" s="85" t="s">
+      <c r="E30" s="70" t="s">
         <v>564</v>
       </c>
-      <c r="F30" s="85" t="s">
+      <c r="F30" s="70" t="s">
         <v>564</v>
       </c>
       <c r="G30" s="38" t="s">
@@ -4394,44 +4394,44 @@
       </c>
       <c r="M30" s="55"/>
     </row>
-    <row r="31" spans="1:13" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="94" t="s">
+    <row r="31" spans="1:13" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="B31" s="95" t="s">
+      <c r="B31" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="95" t="s">
+      <c r="C31" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="96" t="s">
+      <c r="D31" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="E31" s="97" t="s">
+      <c r="E31" s="82" t="s">
         <v>563</v>
       </c>
-      <c r="F31" s="97" t="s">
+      <c r="F31" s="82" t="s">
         <v>539</v>
       </c>
-      <c r="G31" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="H31" s="99">
+      <c r="G31" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="84">
         <v>44568</v>
       </c>
-      <c r="I31" s="99">
+      <c r="I31" s="84">
         <v>44582</v>
       </c>
-      <c r="J31" s="99">
+      <c r="J31" s="84">
         <v>44583</v>
       </c>
-      <c r="K31" s="94" t="s">
+      <c r="K31" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="L31" s="95" t="s">
+      <c r="L31" s="80" t="s">
         <v>282</v>
       </c>
-      <c r="M31" s="100" t="s">
+      <c r="M31" s="85" t="s">
         <v>379</v>
       </c>
     </row>
@@ -4448,10 +4448,10 @@
       <c r="D32" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="E32" s="87" t="s">
+      <c r="E32" s="72" t="s">
         <v>567</v>
       </c>
-      <c r="F32" s="87" t="s">
+      <c r="F32" s="72" t="s">
         <v>566</v>
       </c>
       <c r="G32" s="44" t="s">
@@ -4489,10 +4489,10 @@
       <c r="D33" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="E33" s="85" t="s">
+      <c r="E33" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F33" s="85" t="s">
+      <c r="F33" s="70" t="s">
         <v>560</v>
       </c>
       <c r="G33" s="38" t="s">
@@ -4529,10 +4529,10 @@
       <c r="D34" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="E34" s="85" t="s">
+      <c r="E34" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F34" s="85" t="s">
+      <c r="F34" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G34" s="38" t="s">
@@ -4570,10 +4570,10 @@
       <c r="D35" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="E35" s="85" t="s">
+      <c r="E35" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F35" s="85" t="s">
+      <c r="F35" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G35" s="38" t="s">
@@ -4609,10 +4609,10 @@
       <c r="D36" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="E36" s="85" t="s">
+      <c r="E36" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F36" s="85" t="s">
+      <c r="F36" s="70" t="s">
         <v>559</v>
       </c>
       <c r="G36" s="38" t="s">
@@ -4650,10 +4650,10 @@
       <c r="D37" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="E37" s="85" t="s">
+      <c r="E37" s="70" t="s">
         <v>564</v>
       </c>
-      <c r="F37" s="85" t="s">
+      <c r="F37" s="70" t="s">
         <v>564</v>
       </c>
       <c r="G37" s="38" t="s">
@@ -4691,10 +4691,10 @@
       <c r="D38" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="E38" s="85" t="s">
+      <c r="E38" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F38" s="85" t="s">
+      <c r="F38" s="70" t="s">
         <v>546</v>
       </c>
       <c r="G38" s="38" t="s">
@@ -4732,10 +4732,10 @@
       <c r="D39" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="E39" s="85" t="s">
+      <c r="E39" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F39" s="85" t="s">
+      <c r="F39" s="70" t="s">
         <v>557</v>
       </c>
       <c r="G39" s="38" t="s">
@@ -4772,10 +4772,10 @@
       <c r="D40" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="E40" s="85" t="s">
+      <c r="E40" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F40" s="85" t="s">
+      <c r="F40" s="70" t="s">
         <v>558</v>
       </c>
       <c r="G40" s="38" t="s">
@@ -4811,10 +4811,10 @@
       <c r="D41" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="E41" s="85" t="s">
+      <c r="E41" s="70" t="s">
         <v>561</v>
       </c>
-      <c r="F41" s="85" t="s">
+      <c r="F41" s="70" t="s">
         <v>568</v>
       </c>
       <c r="G41" s="38" t="s">
@@ -4851,10 +4851,10 @@
       <c r="D42" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="85" t="s">
+      <c r="E42" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F42" s="85" t="s">
+      <c r="F42" s="70" t="s">
         <v>551</v>
       </c>
       <c r="G42" s="38" t="s">
@@ -4889,13 +4889,13 @@
       <c r="D43" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="E43" s="85" t="s">
+      <c r="E43" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F43" s="85" t="s">
+      <c r="F43" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="G43" s="81" t="s">
+      <c r="G43" s="66" t="s">
         <v>18</v>
       </c>
       <c r="H43" s="55">
@@ -4928,10 +4928,10 @@
       <c r="D44" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="E44" s="85" t="s">
+      <c r="E44" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F44" s="85" t="s">
+      <c r="F44" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G44" s="38" t="s">
@@ -4967,10 +4967,10 @@
       <c r="D45" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="E45" s="85" t="s">
+      <c r="E45" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F45" s="85" t="s">
+      <c r="F45" s="70" t="s">
         <v>542</v>
       </c>
       <c r="G45" s="38" t="s">
@@ -5006,10 +5006,10 @@
       <c r="D46" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="E46" s="85" t="s">
+      <c r="E46" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F46" s="85" t="s">
+      <c r="F46" s="70" t="s">
         <v>30</v>
       </c>
       <c r="G46" s="38" t="s">
@@ -5045,10 +5045,10 @@
       <c r="D47" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="E47" s="85" t="s">
+      <c r="E47" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F47" s="85" t="s">
+      <c r="F47" s="70" t="s">
         <v>30</v>
       </c>
       <c r="G47" s="38" t="s">
@@ -5084,10 +5084,10 @@
       <c r="D48" s="39" t="s">
         <v>243</v>
       </c>
-      <c r="E48" s="85" t="s">
+      <c r="E48" s="70" t="s">
         <v>555</v>
       </c>
-      <c r="F48" s="85" t="s">
+      <c r="F48" s="70" t="s">
         <v>569</v>
       </c>
       <c r="G48" s="38" t="s">
@@ -5123,10 +5123,10 @@
       <c r="D49" s="39" t="s">
         <v>245</v>
       </c>
-      <c r="E49" s="85" t="s">
+      <c r="E49" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F49" s="85" t="s">
+      <c r="F49" s="70" t="s">
         <v>558</v>
       </c>
       <c r="G49" s="38" t="s">
@@ -5162,10 +5162,10 @@
       <c r="D50" s="39" t="s">
         <v>246</v>
       </c>
-      <c r="E50" s="85" t="s">
+      <c r="E50" s="70" t="s">
         <v>561</v>
       </c>
-      <c r="F50" s="85" t="s">
+      <c r="F50" s="70" t="s">
         <v>568</v>
       </c>
       <c r="G50" s="38" t="s">
@@ -5199,10 +5199,10 @@
       <c r="D51" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="E51" s="85" t="s">
+      <c r="E51" s="70" t="s">
         <v>564</v>
       </c>
-      <c r="F51" s="85" t="s">
+      <c r="F51" s="70" t="s">
         <v>564</v>
       </c>
       <c r="G51" s="38" t="s">
@@ -5238,10 +5238,10 @@
       <c r="D52" s="39" t="s">
         <v>249</v>
       </c>
-      <c r="E52" s="85" t="s">
+      <c r="E52" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F52" s="85" t="s">
+      <c r="F52" s="70" t="s">
         <v>558</v>
       </c>
       <c r="G52" s="38" t="s">
@@ -5275,10 +5275,10 @@
       <c r="D53" s="39" t="s">
         <v>250</v>
       </c>
-      <c r="E53" s="85" t="s">
+      <c r="E53" s="70" t="s">
         <v>570</v>
       </c>
-      <c r="F53" s="85" t="s">
+      <c r="F53" s="70" t="s">
         <v>570</v>
       </c>
       <c r="G53" s="38" t="s">
@@ -5314,10 +5314,10 @@
       <c r="D54" s="39" t="s">
         <v>258</v>
       </c>
-      <c r="E54" s="85" t="s">
+      <c r="E54" s="70" t="s">
         <v>561</v>
       </c>
-      <c r="F54" s="85" t="s">
+      <c r="F54" s="70" t="s">
         <v>568</v>
       </c>
       <c r="G54" s="38" t="s">
@@ -5353,10 +5353,10 @@
       <c r="D55" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="E55" s="85" t="s">
+      <c r="E55" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F55" s="85" t="s">
+      <c r="F55" s="70" t="s">
         <v>551</v>
       </c>
       <c r="G55" s="38" t="s">
@@ -5392,10 +5392,10 @@
       <c r="D56" s="39" t="s">
         <v>261</v>
       </c>
-      <c r="E56" s="85" t="s">
+      <c r="E56" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F56" s="85" t="s">
+      <c r="F56" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G56" s="38" t="s">
@@ -5431,10 +5431,10 @@
       <c r="D57" s="39" t="s">
         <v>262</v>
       </c>
-      <c r="E57" s="85" t="s">
+      <c r="E57" s="70" t="s">
         <v>597</v>
       </c>
-      <c r="F57" s="85" t="s">
+      <c r="F57" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G57" s="38" t="s">
@@ -5470,10 +5470,10 @@
       <c r="D58" s="39" t="s">
         <v>263</v>
       </c>
-      <c r="E58" s="85" t="s">
+      <c r="E58" s="70" t="s">
         <v>457</v>
       </c>
-      <c r="F58" s="85" t="s">
+      <c r="F58" s="70" t="s">
         <v>457</v>
       </c>
       <c r="G58" s="38" t="s">
@@ -5509,10 +5509,10 @@
       <c r="D59" s="39" t="s">
         <v>306</v>
       </c>
-      <c r="E59" s="85" t="s">
+      <c r="E59" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F59" s="85" t="s">
+      <c r="F59" s="70" t="s">
         <v>30</v>
       </c>
       <c r="G59" s="38" t="s">
@@ -5548,10 +5548,10 @@
       <c r="D60" s="39" t="s">
         <v>265</v>
       </c>
-      <c r="E60" s="85" t="s">
+      <c r="E60" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F60" s="85" t="s">
+      <c r="F60" s="70" t="s">
         <v>30</v>
       </c>
       <c r="G60" s="38" t="s">
@@ -5587,10 +5587,10 @@
       <c r="D61" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="E61" s="85" t="s">
+      <c r="E61" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F61" s="85" t="s">
+      <c r="F61" s="70" t="s">
         <v>18</v>
       </c>
       <c r="G61" s="38" t="s">
@@ -5626,10 +5626,10 @@
       <c r="D62" s="39" t="s">
         <v>277</v>
       </c>
-      <c r="E62" s="85" t="s">
+      <c r="E62" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F62" s="85" t="s">
+      <c r="F62" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G62" s="38" t="s">
@@ -5665,10 +5665,10 @@
       <c r="D63" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="E63" s="85" t="s">
+      <c r="E63" s="70" t="s">
         <v>561</v>
       </c>
-      <c r="F63" s="85" t="s">
+      <c r="F63" s="70" t="s">
         <v>561</v>
       </c>
       <c r="G63" s="38" t="s">
@@ -5691,45 +5691,45 @@
       </c>
       <c r="M63" s="55"/>
     </row>
-    <row r="64" spans="1:13" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="94" t="s">
+    <row r="64" spans="1:13" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="B64" s="95" t="s">
+      <c r="B64" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="C64" s="95" t="s">
+      <c r="C64" s="80" t="s">
         <v>242</v>
       </c>
-      <c r="D64" s="96" t="s">
+      <c r="D64" s="81" t="s">
         <v>270</v>
       </c>
-      <c r="E64" s="97" t="s">
+      <c r="E64" s="82" t="s">
         <v>563</v>
       </c>
-      <c r="F64" s="98" t="s">
+      <c r="F64" s="83" t="s">
         <v>539</v>
       </c>
-      <c r="G64" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="H64" s="99">
+      <c r="G64" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H64" s="84">
         <v>44583</v>
       </c>
-      <c r="I64" s="99">
+      <c r="I64" s="84">
         <v>44585</v>
       </c>
-      <c r="J64" s="99">
+      <c r="J64" s="84">
         <f>Tabla1[[#This Row],[FECHA DE CIRUGIA ]]+7</f>
         <v>44592</v>
       </c>
-      <c r="K64" s="94" t="s">
+      <c r="K64" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="L64" s="95" t="s">
+      <c r="L64" s="80" t="s">
         <v>109</v>
       </c>
-      <c r="M64" s="100" t="s">
+      <c r="M64" s="85" t="s">
         <v>380</v>
       </c>
     </row>
@@ -5746,10 +5746,10 @@
       <c r="D65" s="39" t="s">
         <v>271</v>
       </c>
-      <c r="E65" s="85" t="s">
+      <c r="E65" s="70" t="s">
         <v>570</v>
       </c>
-      <c r="F65" s="85" t="s">
+      <c r="F65" s="70" t="s">
         <v>570</v>
       </c>
       <c r="G65" s="38" t="s">
@@ -5785,10 +5785,10 @@
       <c r="D66" s="39" t="s">
         <v>272</v>
       </c>
-      <c r="E66" s="85" t="s">
+      <c r="E66" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F66" s="85" t="s">
+      <c r="F66" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G66" s="38" t="s">
@@ -5825,10 +5825,10 @@
       <c r="D67" s="39" t="s">
         <v>285</v>
       </c>
-      <c r="E67" s="85" t="s">
+      <c r="E67" s="70" t="s">
         <v>595</v>
       </c>
-      <c r="F67" s="85" t="s">
+      <c r="F67" s="70" t="s">
         <v>596</v>
       </c>
       <c r="G67" s="38" t="s">
@@ -5864,10 +5864,10 @@
       <c r="D68" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E68" s="85" t="s">
+      <c r="E68" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F68" s="85" t="s">
+      <c r="F68" s="70" t="s">
         <v>546</v>
       </c>
       <c r="G68" s="38" t="s">
@@ -5903,10 +5903,10 @@
       <c r="D69" s="39" t="s">
         <v>287</v>
       </c>
-      <c r="E69" s="85" t="s">
+      <c r="E69" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F69" s="85" t="s">
+      <c r="F69" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G69" s="38" t="s">
@@ -5943,10 +5943,10 @@
       <c r="D70" s="39" t="s">
         <v>286</v>
       </c>
-      <c r="E70" s="85" t="s">
+      <c r="E70" s="70" t="s">
         <v>564</v>
       </c>
-      <c r="F70" s="85" t="s">
+      <c r="F70" s="70" t="s">
         <v>564</v>
       </c>
       <c r="G70" s="38" t="s">
@@ -5983,10 +5983,10 @@
       <c r="D71" s="39" t="s">
         <v>289</v>
       </c>
-      <c r="E71" s="85" t="s">
+      <c r="E71" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F71" s="85" t="s">
+      <c r="F71" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G71" s="38" t="s">
@@ -6023,10 +6023,10 @@
       <c r="D72" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E72" s="85" t="s">
+      <c r="E72" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F72" s="85" t="s">
+      <c r="F72" s="70" t="s">
         <v>546</v>
       </c>
       <c r="G72" s="38" t="s">
@@ -6063,10 +6063,10 @@
       <c r="D73" s="39" t="s">
         <v>291</v>
       </c>
-      <c r="E73" s="85" t="s">
+      <c r="E73" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F73" s="85" t="s">
+      <c r="F73" s="70" t="s">
         <v>542</v>
       </c>
       <c r="G73" s="38" t="s">
@@ -6103,10 +6103,10 @@
       <c r="D74" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="E74" s="85" t="s">
+      <c r="E74" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F74" s="85" t="s">
+      <c r="F74" s="70" t="s">
         <v>18</v>
       </c>
       <c r="G74" s="38" t="s">
@@ -6144,10 +6144,10 @@
       <c r="D75" s="39" t="s">
         <v>292</v>
       </c>
-      <c r="E75" s="85" t="s">
+      <c r="E75" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F75" s="85" t="s">
+      <c r="F75" s="70" t="s">
         <v>18</v>
       </c>
       <c r="G75" s="38" t="s">
@@ -6185,10 +6185,10 @@
       <c r="D76" s="39" t="s">
         <v>308</v>
       </c>
-      <c r="E76" s="85" t="s">
+      <c r="E76" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F76" s="85" t="s">
+      <c r="F76" s="70" t="s">
         <v>575</v>
       </c>
       <c r="G76" s="38" t="s">
@@ -6226,10 +6226,10 @@
       <c r="D77" s="39" t="s">
         <v>295</v>
       </c>
-      <c r="E77" s="85" t="s">
+      <c r="E77" s="70" t="s">
         <v>457</v>
       </c>
-      <c r="F77" s="85" t="s">
+      <c r="F77" s="70" t="s">
         <v>457</v>
       </c>
       <c r="G77" s="38" t="s">
@@ -6267,10 +6267,10 @@
       <c r="D78" s="39" t="s">
         <v>298</v>
       </c>
-      <c r="E78" s="85" t="s">
+      <c r="E78" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F78" s="85" t="s">
+      <c r="F78" s="70" t="s">
         <v>558</v>
       </c>
       <c r="G78" s="38" t="s">
@@ -6308,10 +6308,10 @@
       <c r="D79" s="39" t="s">
         <v>306</v>
       </c>
-      <c r="E79" s="85" t="s">
+      <c r="E79" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F79" s="85" t="s">
+      <c r="F79" s="70" t="s">
         <v>30</v>
       </c>
       <c r="G79" s="38" t="s">
@@ -6349,10 +6349,10 @@
       <c r="D80" s="39" t="s">
         <v>307</v>
       </c>
-      <c r="E80" s="85" t="s">
+      <c r="E80" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F80" s="85" t="s">
+      <c r="F80" s="70" t="s">
         <v>30</v>
       </c>
       <c r="G80" s="38" t="s">
@@ -6389,10 +6389,10 @@
       <c r="D81" s="39" t="s">
         <v>309</v>
       </c>
-      <c r="E81" s="85" t="s">
+      <c r="E81" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F81" s="85" t="s">
+      <c r="F81" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G81" s="38" t="s">
@@ -6429,10 +6429,10 @@
       <c r="D82" s="39" t="s">
         <v>311</v>
       </c>
-      <c r="E82" s="85" t="s">
+      <c r="E82" s="70" t="s">
         <v>457</v>
       </c>
-      <c r="F82" s="85" t="s">
+      <c r="F82" s="70" t="s">
         <v>457</v>
       </c>
       <c r="G82" s="38" t="s">
@@ -6470,10 +6470,10 @@
       <c r="D83" s="39" t="s">
         <v>312</v>
       </c>
-      <c r="E83" s="85" t="s">
+      <c r="E83" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F83" s="85" t="s">
+      <c r="F83" s="70" t="s">
         <v>559</v>
       </c>
       <c r="G83" s="38" t="s">
@@ -6511,10 +6511,10 @@
       <c r="D84" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E84" s="85" t="s">
+      <c r="E84" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F84" s="85" t="s">
+      <c r="F84" s="70" t="s">
         <v>542</v>
       </c>
       <c r="G84" s="38" t="s">
@@ -6552,10 +6552,10 @@
       <c r="D85" s="39" t="s">
         <v>317</v>
       </c>
-      <c r="E85" s="85" t="s">
+      <c r="E85" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F85" s="85" t="s">
+      <c r="F85" s="70" t="s">
         <v>18</v>
       </c>
       <c r="G85" s="38" t="s">
@@ -6593,10 +6593,10 @@
       <c r="D86" s="39" t="s">
         <v>319</v>
       </c>
-      <c r="E86" s="85" t="s">
+      <c r="E86" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F86" s="85" t="s">
+      <c r="F86" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G86" s="38" t="s">
@@ -6634,10 +6634,10 @@
       <c r="D87" s="39" t="s">
         <v>321</v>
       </c>
-      <c r="E87" s="85" t="s">
+      <c r="E87" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F87" s="85" t="s">
+      <c r="F87" s="70" t="s">
         <v>593</v>
       </c>
       <c r="G87" s="38" t="s">
@@ -6675,10 +6675,10 @@
       <c r="D88" s="39" t="s">
         <v>322</v>
       </c>
-      <c r="E88" s="85" t="s">
+      <c r="E88" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F88" s="85" t="s">
+      <c r="F88" s="70" t="s">
         <v>18</v>
       </c>
       <c r="G88" s="38" t="s">
@@ -6716,10 +6716,10 @@
       <c r="D89" s="39" t="s">
         <v>326</v>
       </c>
-      <c r="E89" s="85" t="s">
+      <c r="E89" s="70" t="s">
         <v>561</v>
       </c>
-      <c r="F89" s="85" t="s">
+      <c r="F89" s="70" t="s">
         <v>561</v>
       </c>
       <c r="G89" s="38" t="s">
@@ -6757,10 +6757,10 @@
       <c r="D90" s="39" t="s">
         <v>331</v>
       </c>
-      <c r="E90" s="85" t="s">
+      <c r="E90" s="70" t="s">
         <v>328</v>
       </c>
-      <c r="F90" s="85" t="s">
+      <c r="F90" s="70" t="s">
         <v>328</v>
       </c>
       <c r="G90" s="38" t="s">
@@ -6798,10 +6798,10 @@
       <c r="D91" s="39" t="s">
         <v>323</v>
       </c>
-      <c r="E91" s="85" t="s">
+      <c r="E91" s="70" t="s">
         <v>457</v>
       </c>
-      <c r="F91" s="85" t="s">
+      <c r="F91" s="70" t="s">
         <v>457</v>
       </c>
       <c r="G91" s="38" t="s">
@@ -6839,10 +6839,10 @@
       <c r="D92" s="39" t="s">
         <v>324</v>
       </c>
-      <c r="E92" s="85" t="s">
+      <c r="E92" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F92" s="85" t="s">
+      <c r="F92" s="70" t="s">
         <v>18</v>
       </c>
       <c r="G92" s="38" t="s">
@@ -6880,10 +6880,10 @@
       <c r="D93" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E93" s="85" t="s">
+      <c r="E93" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F93" s="85" t="s">
+      <c r="F93" s="70" t="s">
         <v>560</v>
       </c>
       <c r="G93" s="38" t="s">
@@ -6921,10 +6921,10 @@
       <c r="D94" s="39" t="s">
         <v>325</v>
       </c>
-      <c r="E94" s="85" t="s">
+      <c r="E94" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F94" s="85" t="s">
+      <c r="F94" s="70" t="s">
         <v>18</v>
       </c>
       <c r="G94" s="38" t="s">
@@ -6962,10 +6962,10 @@
       <c r="D95" s="39" t="s">
         <v>330</v>
       </c>
-      <c r="E95" s="85" t="s">
+      <c r="E95" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F95" s="85" t="s">
+      <c r="F95" s="70" t="s">
         <v>558</v>
       </c>
       <c r="G95" s="38" t="s">
@@ -7003,10 +7003,10 @@
       <c r="D96" s="39" t="s">
         <v>334</v>
       </c>
-      <c r="E96" s="85" t="s">
+      <c r="E96" s="70" t="s">
         <v>457</v>
       </c>
-      <c r="F96" s="85" t="s">
+      <c r="F96" s="70" t="s">
         <v>457</v>
       </c>
       <c r="G96" s="38" t="s">
@@ -7043,10 +7043,10 @@
       <c r="D97" s="39" t="s">
         <v>353</v>
       </c>
-      <c r="E97" s="85" t="s">
+      <c r="E97" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F97" s="85" t="s">
+      <c r="F97" s="70" t="s">
         <v>592</v>
       </c>
       <c r="G97" s="38" t="s">
@@ -7084,10 +7084,10 @@
       <c r="D98" s="39" t="s">
         <v>337</v>
       </c>
-      <c r="E98" s="85" t="s">
+      <c r="E98" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F98" s="85" t="s">
+      <c r="F98" s="70" t="s">
         <v>546</v>
       </c>
       <c r="G98" s="38" t="s">
@@ -7125,10 +7125,10 @@
       <c r="D99" s="39" t="s">
         <v>339</v>
       </c>
-      <c r="E99" s="85" t="s">
+      <c r="E99" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F99" s="85" t="s">
+      <c r="F99" s="70" t="s">
         <v>557</v>
       </c>
       <c r="G99" s="38" t="s">
@@ -7166,10 +7166,10 @@
       <c r="D100" s="50" t="s">
         <v>338</v>
       </c>
-      <c r="E100" s="89" t="s">
+      <c r="E100" s="74" t="s">
         <v>538</v>
       </c>
-      <c r="F100" s="89" t="s">
+      <c r="F100" s="74" t="s">
         <v>538</v>
       </c>
       <c r="G100" s="52" t="s">
@@ -7208,10 +7208,10 @@
       <c r="D101" s="39" t="s">
         <v>349</v>
       </c>
-      <c r="E101" s="85" t="s">
+      <c r="E101" s="70" t="s">
         <v>561</v>
       </c>
-      <c r="F101" s="85" t="s">
+      <c r="F101" s="70" t="s">
         <v>561</v>
       </c>
       <c r="G101" s="38" t="s">
@@ -7248,10 +7248,10 @@
       <c r="D102" s="39" t="s">
         <v>343</v>
       </c>
-      <c r="E102" s="85" t="s">
+      <c r="E102" s="70" t="s">
         <v>591</v>
       </c>
-      <c r="F102" s="85" t="s">
+      <c r="F102" s="70" t="s">
         <v>590</v>
       </c>
       <c r="G102" s="38" t="s">
@@ -7289,10 +7289,10 @@
       <c r="D103" s="39" t="s">
         <v>350</v>
       </c>
-      <c r="E103" s="85" t="s">
+      <c r="E103" s="70" t="s">
         <v>561</v>
       </c>
-      <c r="F103" s="85" t="s">
+      <c r="F103" s="70" t="s">
         <v>561</v>
       </c>
       <c r="G103" s="38" t="s">
@@ -7330,10 +7330,10 @@
       <c r="D104" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="E104" s="85" t="s">
+      <c r="E104" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F104" s="85" t="s">
+      <c r="F104" s="70" t="s">
         <v>589</v>
       </c>
       <c r="G104" s="38" t="s">
@@ -7370,10 +7370,10 @@
       <c r="D105" s="39" t="s">
         <v>346</v>
       </c>
-      <c r="E105" s="85" t="s">
+      <c r="E105" s="70" t="s">
         <v>457</v>
       </c>
-      <c r="F105" s="85" t="s">
+      <c r="F105" s="70" t="s">
         <v>457</v>
       </c>
       <c r="G105" s="38" t="s">
@@ -7411,10 +7411,10 @@
       <c r="D106" s="39" t="s">
         <v>351</v>
       </c>
-      <c r="E106" s="85" t="s">
+      <c r="E106" s="70" t="s">
         <v>457</v>
       </c>
-      <c r="F106" s="85" t="s">
+      <c r="F106" s="70" t="s">
         <v>457</v>
       </c>
       <c r="G106" s="38" t="s">
@@ -7452,10 +7452,10 @@
       <c r="D107" s="39" t="s">
         <v>377</v>
       </c>
-      <c r="E107" s="85" t="s">
+      <c r="E107" s="70" t="s">
         <v>561</v>
       </c>
-      <c r="F107" s="85" t="s">
+      <c r="F107" s="70" t="s">
         <v>561</v>
       </c>
       <c r="G107" s="38" t="s">
@@ -7493,10 +7493,10 @@
       <c r="D108" s="39" t="s">
         <v>378</v>
       </c>
-      <c r="E108" s="85" t="s">
+      <c r="E108" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F108" s="85" t="s">
+      <c r="F108" s="70" t="s">
         <v>587</v>
       </c>
       <c r="G108" s="38" t="s">
@@ -7534,10 +7534,10 @@
       <c r="D109" s="39" t="s">
         <v>373</v>
       </c>
-      <c r="E109" s="85" t="s">
+      <c r="E109" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F109" s="85" t="s">
+      <c r="F109" s="70" t="s">
         <v>551</v>
       </c>
       <c r="G109" s="38" t="s">
@@ -7575,10 +7575,10 @@
       <c r="D110" s="39" t="s">
         <v>374</v>
       </c>
-      <c r="E110" s="85" t="s">
+      <c r="E110" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F110" s="85" t="s">
+      <c r="F110" s="70" t="s">
         <v>587</v>
       </c>
       <c r="G110" s="38" t="s">
@@ -7616,10 +7616,10 @@
       <c r="D111" s="39" t="s">
         <v>375</v>
       </c>
-      <c r="E111" s="85" t="s">
+      <c r="E111" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F111" s="85" t="s">
+      <c r="F111" s="70" t="s">
         <v>558</v>
       </c>
       <c r="G111" s="38" t="s">
@@ -7657,10 +7657,10 @@
       <c r="D112" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="E112" s="85" t="s">
+      <c r="E112" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F112" s="85" t="s">
+      <c r="F112" s="70" t="s">
         <v>575</v>
       </c>
       <c r="G112" s="38" t="s">
@@ -7698,10 +7698,10 @@
       <c r="D113" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E113" s="85" t="s">
+      <c r="E113" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F113" s="85" t="s">
+      <c r="F113" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G113" s="38" t="s">
@@ -7739,10 +7739,10 @@
       <c r="D114" s="39" t="s">
         <v>382</v>
       </c>
-      <c r="E114" s="85" t="s">
+      <c r="E114" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F114" s="85" t="s">
+      <c r="F114" s="70" t="s">
         <v>30</v>
       </c>
       <c r="G114" s="38" t="s">
@@ -7780,10 +7780,10 @@
       <c r="D115" s="39" t="s">
         <v>384</v>
       </c>
-      <c r="E115" s="85" t="s">
+      <c r="E115" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F115" s="85" t="s">
+      <c r="F115" s="70" t="s">
         <v>542</v>
       </c>
       <c r="G115" s="38" t="s">
@@ -7821,10 +7821,10 @@
       <c r="D116" s="39" t="s">
         <v>385</v>
       </c>
-      <c r="E116" s="85" t="s">
+      <c r="E116" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F116" s="85" t="s">
+      <c r="F116" s="70" t="s">
         <v>574</v>
       </c>
       <c r="G116" s="38" t="s">
@@ -7862,10 +7862,10 @@
       <c r="D117" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E117" s="85" t="s">
+      <c r="E117" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F117" s="85" t="s">
+      <c r="F117" s="70" t="s">
         <v>578</v>
       </c>
       <c r="G117" s="38" t="s">
@@ -7903,13 +7903,13 @@
       <c r="D118" s="39" t="s">
         <v>388</v>
       </c>
-      <c r="E118" s="85" t="s">
+      <c r="E118" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F118" s="85" t="s">
+      <c r="F118" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="G118" s="80" t="s">
+      <c r="G118" s="65" t="s">
         <v>18</v>
       </c>
       <c r="H118" s="55">
@@ -7944,13 +7944,13 @@
       <c r="D119" s="54" t="s">
         <v>392</v>
       </c>
-      <c r="E119" s="90" t="s">
+      <c r="E119" s="75" t="s">
         <v>544</v>
       </c>
-      <c r="F119" s="90" t="s">
+      <c r="F119" s="75" t="s">
         <v>544</v>
       </c>
-      <c r="G119" s="82" t="s">
+      <c r="G119" s="67" t="s">
         <v>391</v>
       </c>
       <c r="H119" s="61">
@@ -7985,10 +7985,10 @@
       <c r="D120" s="45" t="s">
         <v>400</v>
       </c>
-      <c r="E120" s="87" t="s">
+      <c r="E120" s="72" t="s">
         <v>585</v>
       </c>
-      <c r="F120" s="87" t="s">
+      <c r="F120" s="72" t="s">
         <v>588</v>
       </c>
       <c r="G120" s="38" t="s">
@@ -8026,10 +8026,10 @@
       <c r="D121" s="39" t="s">
         <v>432</v>
       </c>
-      <c r="E121" s="85" t="s">
+      <c r="E121" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F121" s="85" t="s">
+      <c r="F121" s="70" t="s">
         <v>30</v>
       </c>
       <c r="G121" s="38" t="s">
@@ -8067,10 +8067,10 @@
       <c r="D122" s="39" t="s">
         <v>430</v>
       </c>
-      <c r="E122" s="85" t="s">
+      <c r="E122" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F122" s="85" t="s">
+      <c r="F122" s="70" t="s">
         <v>538</v>
       </c>
       <c r="G122" s="38" t="s">
@@ -8108,10 +8108,10 @@
       <c r="D123" s="39" t="s">
         <v>398</v>
       </c>
-      <c r="E123" s="85" t="s">
+      <c r="E123" s="70" t="s">
         <v>583</v>
       </c>
-      <c r="F123" s="85" t="s">
+      <c r="F123" s="70" t="s">
         <v>583</v>
       </c>
       <c r="G123" s="38" t="s">
@@ -8149,10 +8149,10 @@
       <c r="D124" s="39" t="s">
         <v>424</v>
       </c>
-      <c r="E124" s="85" t="s">
+      <c r="E124" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F124" s="85" t="s">
+      <c r="F124" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G124" s="38" t="s">
@@ -8190,10 +8190,10 @@
       <c r="D125" s="39" t="s">
         <v>428</v>
       </c>
-      <c r="E125" s="85" t="s">
+      <c r="E125" s="70" t="s">
         <v>585</v>
       </c>
-      <c r="F125" s="85" t="s">
+      <c r="F125" s="70" t="s">
         <v>586</v>
       </c>
       <c r="G125" s="38" t="s">
@@ -8233,10 +8233,10 @@
       <c r="D126" s="39" t="s">
         <v>425</v>
       </c>
-      <c r="E126" s="85" t="s">
+      <c r="E126" s="70" t="s">
         <v>457</v>
       </c>
-      <c r="F126" s="85" t="s">
+      <c r="F126" s="70" t="s">
         <v>457</v>
       </c>
       <c r="G126" s="38" t="s">
@@ -8274,10 +8274,10 @@
       <c r="D127" s="39" t="s">
         <v>431</v>
       </c>
-      <c r="E127" s="85" t="s">
+      <c r="E127" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F127" s="85" t="s">
+      <c r="F127" s="70" t="s">
         <v>18</v>
       </c>
       <c r="G127" s="38" t="s">
@@ -8315,10 +8315,10 @@
       <c r="D128" s="39" t="s">
         <v>433</v>
       </c>
-      <c r="E128" s="85" t="s">
+      <c r="E128" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F128" s="85" t="s">
+      <c r="F128" s="70" t="s">
         <v>559</v>
       </c>
       <c r="G128" s="38" t="s">
@@ -8356,10 +8356,10 @@
       <c r="D129" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E129" s="85" t="s">
+      <c r="E129" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F129" s="85" t="s">
+      <c r="F129" s="70" t="s">
         <v>542</v>
       </c>
       <c r="G129" s="38" t="s">
@@ -8397,10 +8397,10 @@
       <c r="D130" s="39" t="s">
         <v>434</v>
       </c>
-      <c r="E130" s="85" t="s">
+      <c r="E130" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F130" s="85" t="s">
+      <c r="F130" s="70" t="s">
         <v>540</v>
       </c>
       <c r="G130" s="38" t="s">
@@ -8437,10 +8437,10 @@
       <c r="D131" s="39" t="s">
         <v>435</v>
       </c>
-      <c r="E131" s="85" t="s">
+      <c r="E131" s="70" t="s">
         <v>449</v>
       </c>
-      <c r="F131" s="85" t="s">
+      <c r="F131" s="70" t="s">
         <v>449</v>
       </c>
       <c r="G131" s="38" t="s">
@@ -8477,10 +8477,10 @@
       <c r="D132" s="62" t="s">
         <v>436</v>
       </c>
-      <c r="E132" s="91" t="s">
+      <c r="E132" s="76" t="s">
         <v>538</v>
       </c>
-      <c r="F132" s="91" t="s">
+      <c r="F132" s="76" t="s">
         <v>559</v>
       </c>
       <c r="G132" s="38" t="s">
@@ -8518,10 +8518,10 @@
       <c r="D133" s="39" t="s">
         <v>439</v>
       </c>
-      <c r="E133" s="85" t="s">
+      <c r="E133" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F133" s="85" t="s">
+      <c r="F133" s="70" t="s">
         <v>560</v>
       </c>
       <c r="G133" s="38" t="s">
@@ -8559,10 +8559,10 @@
       <c r="D134" s="39" t="s">
         <v>437</v>
       </c>
-      <c r="E134" s="85" t="s">
+      <c r="E134" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F134" s="85" t="s">
+      <c r="F134" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G134" s="38" t="s">
@@ -8600,10 +8600,10 @@
       <c r="D135" s="39" t="s">
         <v>441</v>
       </c>
-      <c r="E135" s="85" t="s">
+      <c r="E135" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F135" s="85" t="s">
+      <c r="F135" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G135" s="38" t="s">
@@ -8641,10 +8641,10 @@
       <c r="D136" s="39" t="s">
         <v>452</v>
       </c>
-      <c r="E136" s="85" t="s">
+      <c r="E136" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F136" s="85" t="s">
+      <c r="F136" s="70" t="s">
         <v>578</v>
       </c>
       <c r="G136" s="38" t="s">
@@ -8682,10 +8682,10 @@
       <c r="D137" s="39" t="s">
         <v>453</v>
       </c>
-      <c r="E137" s="85" t="s">
+      <c r="E137" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F137" s="85" t="s">
+      <c r="F137" s="70" t="s">
         <v>540</v>
       </c>
       <c r="G137" s="38" t="s">
@@ -8723,10 +8723,10 @@
       <c r="D138" s="39" t="s">
         <v>454</v>
       </c>
-      <c r="E138" s="85" t="s">
+      <c r="E138" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F138" s="85" t="s">
+      <c r="F138" s="70" t="s">
         <v>540</v>
       </c>
       <c r="G138" s="38" t="s">
@@ -8764,10 +8764,10 @@
       <c r="D139" s="39" t="s">
         <v>455</v>
       </c>
-      <c r="E139" s="85" t="s">
+      <c r="E139" s="70" t="s">
         <v>584</v>
       </c>
-      <c r="F139" s="85" t="s">
+      <c r="F139" s="70" t="s">
         <v>584</v>
       </c>
       <c r="G139" s="38" t="s">
@@ -8805,10 +8805,10 @@
       <c r="D140" s="39" t="s">
         <v>457</v>
       </c>
-      <c r="E140" s="85" t="s">
+      <c r="E140" s="70" t="s">
         <v>583</v>
       </c>
-      <c r="F140" s="85" t="s">
+      <c r="F140" s="70" t="s">
         <v>583</v>
       </c>
       <c r="G140" s="38" t="s">
@@ -8842,10 +8842,10 @@
       <c r="D141" s="39" t="s">
         <v>460</v>
       </c>
-      <c r="E141" s="85" t="s">
+      <c r="E141" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F141" s="85" t="s">
+      <c r="F141" s="70" t="s">
         <v>559</v>
       </c>
       <c r="G141" s="38" t="s">
@@ -8883,10 +8883,10 @@
       <c r="D142" s="39" t="s">
         <v>461</v>
       </c>
-      <c r="E142" s="85" t="s">
+      <c r="E142" s="70" t="s">
         <v>582</v>
       </c>
-      <c r="F142" s="85" t="s">
+      <c r="F142" s="70" t="s">
         <v>542</v>
       </c>
       <c r="G142" s="38" t="s">
@@ -8924,10 +8924,10 @@
       <c r="D143" s="39" t="s">
         <v>463</v>
       </c>
-      <c r="E143" s="85" t="s">
+      <c r="E143" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F143" s="85" t="s">
+      <c r="F143" s="70" t="s">
         <v>558</v>
       </c>
       <c r="G143" s="38" t="s">
@@ -8965,10 +8965,10 @@
       <c r="D144" s="39" t="s">
         <v>312</v>
       </c>
-      <c r="E144" s="85" t="s">
+      <c r="E144" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F144" s="85" t="s">
+      <c r="F144" s="70" t="s">
         <v>18</v>
       </c>
       <c r="G144" s="38" t="s">
@@ -9006,10 +9006,10 @@
       <c r="D145" s="39" t="s">
         <v>480</v>
       </c>
-      <c r="E145" s="85" t="s">
+      <c r="E145" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F145" s="85" t="s">
+      <c r="F145" s="70" t="s">
         <v>574</v>
       </c>
       <c r="G145" s="38" t="s">
@@ -9047,10 +9047,10 @@
       <c r="D146" s="39" t="s">
         <v>478</v>
       </c>
-      <c r="E146" s="85" t="s">
+      <c r="E146" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F146" s="85" t="s">
+      <c r="F146" s="70" t="s">
         <v>551</v>
       </c>
       <c r="G146" s="38" t="s">
@@ -9088,10 +9088,10 @@
       <c r="D147" s="39" t="s">
         <v>466</v>
       </c>
-      <c r="E147" s="85" t="s">
+      <c r="E147" s="70" t="s">
         <v>580</v>
       </c>
-      <c r="F147" s="85" t="s">
+      <c r="F147" s="70" t="s">
         <v>581</v>
       </c>
       <c r="G147" s="38" t="s">
@@ -9129,10 +9129,10 @@
       <c r="D148" s="39" t="s">
         <v>469</v>
       </c>
-      <c r="E148" s="85" t="s">
+      <c r="E148" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F148" s="85" t="s">
+      <c r="F148" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G148" s="38" t="s">
@@ -9170,10 +9170,10 @@
       <c r="D149" s="39" t="s">
         <v>471</v>
       </c>
-      <c r="E149" s="85" t="s">
+      <c r="E149" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F149" s="85" t="s">
+      <c r="F149" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G149" s="38" t="s">
@@ -9211,10 +9211,10 @@
       <c r="D150" s="39" t="s">
         <v>525</v>
       </c>
-      <c r="E150" s="85" t="s">
+      <c r="E150" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F150" s="85" t="s">
+      <c r="F150" s="70" t="s">
         <v>578</v>
       </c>
       <c r="G150" s="38" t="s">
@@ -9252,10 +9252,10 @@
       <c r="D151" s="39" t="s">
         <v>474</v>
       </c>
-      <c r="E151" s="85" t="s">
+      <c r="E151" s="70" t="s">
         <v>579</v>
       </c>
-      <c r="F151" s="85" t="s">
+      <c r="F151" s="70" t="s">
         <v>558</v>
       </c>
       <c r="G151" s="38" t="s">
@@ -9293,10 +9293,10 @@
       <c r="D152" s="39" t="s">
         <v>476</v>
       </c>
-      <c r="E152" s="85" t="s">
+      <c r="E152" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F152" s="85" t="s">
+      <c r="F152" s="70" t="s">
         <v>30</v>
       </c>
       <c r="G152" s="38" t="s">
@@ -9334,10 +9334,10 @@
       <c r="D153" s="62" t="s">
         <v>484</v>
       </c>
-      <c r="E153" s="85" t="s">
+      <c r="E153" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F153" s="85" t="s">
+      <c r="F153" s="70" t="s">
         <v>30</v>
       </c>
       <c r="G153" s="38" t="s">
@@ -9374,10 +9374,10 @@
       <c r="D154" s="39" t="s">
         <v>487</v>
       </c>
-      <c r="E154" s="85" t="s">
+      <c r="E154" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F154" s="85" t="s">
+      <c r="F154" s="70" t="s">
         <v>30</v>
       </c>
       <c r="G154" s="38" t="s">
@@ -9414,10 +9414,10 @@
       <c r="D155" s="62" t="s">
         <v>486</v>
       </c>
-      <c r="E155" s="91" t="s">
+      <c r="E155" s="76" t="s">
         <v>544</v>
       </c>
-      <c r="F155" s="91" t="s">
+      <c r="F155" s="76" t="s">
         <v>559</v>
       </c>
       <c r="G155" s="38" t="s">
@@ -9455,10 +9455,10 @@
       <c r="D156" s="39" t="s">
         <v>514</v>
       </c>
-      <c r="E156" s="85" t="s">
+      <c r="E156" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="F156" s="85" t="s">
+      <c r="F156" s="70" t="s">
         <v>578</v>
       </c>
       <c r="G156" s="38" t="s">
@@ -9496,10 +9496,10 @@
       <c r="D157" s="39" t="s">
         <v>512</v>
       </c>
-      <c r="E157" s="85" t="s">
+      <c r="E157" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F157" s="85" t="s">
+      <c r="F157" s="70" t="s">
         <v>546</v>
       </c>
       <c r="G157" s="38" t="s">
@@ -9537,10 +9537,10 @@
       <c r="D158" s="39" t="s">
         <v>497</v>
       </c>
-      <c r="E158" s="85" t="s">
+      <c r="E158" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F158" s="85" t="s">
+      <c r="F158" s="70" t="s">
         <v>575</v>
       </c>
       <c r="G158" s="38" t="s">
@@ -9578,10 +9578,10 @@
       <c r="D159" s="39" t="s">
         <v>511</v>
       </c>
-      <c r="E159" s="85" t="s">
+      <c r="E159" s="70" t="s">
         <v>561</v>
       </c>
-      <c r="F159" s="85" t="s">
+      <c r="F159" s="70" t="s">
         <v>561</v>
       </c>
       <c r="G159" s="38" t="s">
@@ -9615,10 +9615,10 @@
       <c r="D160" s="39" t="s">
         <v>499</v>
       </c>
-      <c r="E160" s="85" t="s">
+      <c r="E160" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F160" s="85" t="s">
+      <c r="F160" s="70" t="s">
         <v>560</v>
       </c>
       <c r="G160" s="38" t="s">
@@ -9656,10 +9656,10 @@
       <c r="D161" s="39" t="s">
         <v>500</v>
       </c>
-      <c r="E161" s="85" t="s">
+      <c r="E161" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F161" s="85" t="s">
+      <c r="F161" s="70" t="s">
         <v>577</v>
       </c>
       <c r="G161" s="38" t="s">
@@ -9697,10 +9697,10 @@
       <c r="D162" s="39" t="s">
         <v>501</v>
       </c>
-      <c r="E162" s="85" t="s">
+      <c r="E162" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F162" s="85" t="s">
+      <c r="F162" s="70" t="s">
         <v>540</v>
       </c>
       <c r="G162" s="38" t="s">
@@ -9738,10 +9738,10 @@
       <c r="D163" s="39" t="s">
         <v>510</v>
       </c>
-      <c r="E163" s="85" t="s">
+      <c r="E163" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F163" s="85" t="s">
+      <c r="F163" s="70" t="s">
         <v>30</v>
       </c>
       <c r="G163" s="38" t="s">
@@ -9779,10 +9779,10 @@
       <c r="D164" s="39" t="s">
         <v>505</v>
       </c>
-      <c r="E164" s="85" t="s">
+      <c r="E164" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F164" s="85" t="s">
+      <c r="F164" s="70" t="s">
         <v>557</v>
       </c>
       <c r="G164" s="38" t="s">
@@ -9820,10 +9820,10 @@
       <c r="D165" s="39" t="s">
         <v>520</v>
       </c>
-      <c r="E165" s="85" t="s">
+      <c r="E165" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F165" s="85" t="s">
+      <c r="F165" s="70" t="s">
         <v>574</v>
       </c>
       <c r="G165" s="38" t="s">
@@ -9857,10 +9857,10 @@
       <c r="D166" s="39" t="s">
         <v>516</v>
       </c>
-      <c r="E166" s="85" t="s">
+      <c r="E166" s="70" t="s">
         <v>561</v>
       </c>
-      <c r="F166" s="85" t="s">
+      <c r="F166" s="70" t="s">
         <v>561</v>
       </c>
       <c r="G166" s="38" t="s">
@@ -9898,10 +9898,10 @@
       <c r="D167" s="39" t="s">
         <v>522</v>
       </c>
-      <c r="E167" s="85" t="s">
+      <c r="E167" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F167" s="85" t="s">
+      <c r="F167" s="70" t="s">
         <v>575</v>
       </c>
       <c r="G167" s="38" t="s">
@@ -9935,10 +9935,10 @@
       <c r="D168" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E168" s="85" t="s">
+      <c r="E168" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F168" s="85" t="s">
+      <c r="F168" s="70" t="s">
         <v>576</v>
       </c>
       <c r="G168" s="38" t="s">
@@ -9976,10 +9976,10 @@
       <c r="D169" s="39" t="s">
         <v>527</v>
       </c>
-      <c r="E169" s="85" t="s">
+      <c r="E169" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F169" s="85" t="s">
+      <c r="F169" s="70" t="s">
         <v>18</v>
       </c>
       <c r="G169" s="38" t="s">
@@ -10015,10 +10015,10 @@
       <c r="D170" s="63" t="s">
         <v>536</v>
       </c>
-      <c r="E170" s="85" t="s">
+      <c r="E170" s="70" t="s">
         <v>537</v>
       </c>
-      <c r="F170" s="85" t="s">
+      <c r="F170" s="70" t="s">
         <v>539</v>
       </c>
       <c r="G170" s="38" t="s">
@@ -10051,10 +10051,10 @@
       <c r="D171" s="39" t="s">
         <v>535</v>
       </c>
-      <c r="E171" s="85" t="s">
+      <c r="E171" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F171" s="85" t="s">
+      <c r="F171" s="70" t="s">
         <v>540</v>
       </c>
       <c r="G171" s="38" t="s">
@@ -10087,10 +10087,10 @@
       <c r="D172" s="39" t="s">
         <v>541</v>
       </c>
-      <c r="E172" s="85" t="s">
+      <c r="E172" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F172" s="85" t="s">
+      <c r="F172" s="70" t="s">
         <v>542</v>
       </c>
       <c r="G172" s="38" t="s">
@@ -10127,10 +10127,10 @@
       <c r="D173" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E173" s="85" t="s">
+      <c r="E173" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F173" s="85" t="s">
+      <c r="F173" s="70" t="s">
         <v>545</v>
       </c>
       <c r="G173" s="38" t="s">
@@ -10164,10 +10164,10 @@
       <c r="D174" s="39" t="s">
         <v>572</v>
       </c>
-      <c r="E174" s="85" t="s">
+      <c r="E174" s="70" t="s">
         <v>538</v>
       </c>
-      <c r="F174" s="85" t="s">
+      <c r="F174" s="70" t="s">
         <v>540</v>
       </c>
       <c r="G174" s="38" t="s">
@@ -10201,10 +10201,10 @@
       <c r="D175" s="39" t="s">
         <v>548</v>
       </c>
-      <c r="E175" s="85" t="s">
+      <c r="E175" s="70" t="s">
         <v>544</v>
       </c>
-      <c r="F175" s="85" t="s">
+      <c r="F175" s="70" t="s">
         <v>546</v>
       </c>
       <c r="G175" s="38" t="s">
@@ -10238,10 +10238,10 @@
       <c r="D176" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="E176" s="85" t="s">
+      <c r="E176" s="70" t="s">
         <v>573</v>
       </c>
-      <c r="F176" s="85" t="s">
+      <c r="F176" s="70" t="s">
         <v>573</v>
       </c>
       <c r="G176" s="38" t="s">
@@ -10267,8 +10267,8 @@
       <c r="B177" s="39"/>
       <c r="C177" s="39"/>
       <c r="D177" s="39"/>
-      <c r="E177" s="85"/>
-      <c r="F177" s="85"/>
+      <c r="E177" s="70"/>
+      <c r="F177" s="70"/>
       <c r="G177" s="38"/>
       <c r="H177" s="55"/>
       <c r="I177" s="55"/>
@@ -10282,8 +10282,8 @@
       <c r="B178" s="39"/>
       <c r="C178" s="39"/>
       <c r="D178" s="39"/>
-      <c r="E178" s="85"/>
-      <c r="F178" s="85"/>
+      <c r="E178" s="70"/>
+      <c r="F178" s="70"/>
       <c r="G178" s="38"/>
       <c r="H178" s="55"/>
       <c r="I178" s="55"/>
@@ -10297,8 +10297,8 @@
       <c r="B179" s="39"/>
       <c r="C179" s="39"/>
       <c r="D179" s="39"/>
-      <c r="E179" s="85"/>
-      <c r="F179" s="85"/>
+      <c r="E179" s="70"/>
+      <c r="F179" s="70"/>
       <c r="G179" s="38"/>
       <c r="H179" s="55"/>
       <c r="I179" s="55"/>
@@ -10312,8 +10312,8 @@
       <c r="B180" s="39"/>
       <c r="C180" s="39"/>
       <c r="D180" s="39"/>
-      <c r="E180" s="85"/>
-      <c r="F180" s="85"/>
+      <c r="E180" s="70"/>
+      <c r="F180" s="70"/>
       <c r="G180" s="38"/>
       <c r="H180" s="55"/>
       <c r="I180" s="55"/>
@@ -10327,8 +10327,8 @@
       <c r="B181" s="39"/>
       <c r="C181" s="39"/>
       <c r="D181" s="39"/>
-      <c r="E181" s="85"/>
-      <c r="F181" s="85"/>
+      <c r="E181" s="70"/>
+      <c r="F181" s="70"/>
       <c r="G181" s="38"/>
       <c r="H181" s="55"/>
       <c r="I181" s="55"/>
@@ -10342,8 +10342,8 @@
       <c r="B182" s="39"/>
       <c r="C182" s="39"/>
       <c r="D182" s="39"/>
-      <c r="E182" s="85"/>
-      <c r="F182" s="85"/>
+      <c r="E182" s="70"/>
+      <c r="F182" s="70"/>
       <c r="G182" s="38"/>
       <c r="H182" s="55"/>
       <c r="I182" s="55"/>
@@ -10357,8 +10357,8 @@
       <c r="B183" s="39"/>
       <c r="C183" s="39"/>
       <c r="D183" s="39"/>
-      <c r="E183" s="85"/>
-      <c r="F183" s="85"/>
+      <c r="E183" s="70"/>
+      <c r="F183" s="70"/>
       <c r="G183" s="38"/>
       <c r="H183" s="55"/>
       <c r="I183" s="55"/>
@@ -10372,8 +10372,8 @@
       <c r="B184" s="34"/>
       <c r="C184" s="34"/>
       <c r="D184" s="34"/>
-      <c r="E184" s="92"/>
-      <c r="F184" s="92"/>
+      <c r="E184" s="77"/>
+      <c r="F184" s="77"/>
       <c r="G184" s="1"/>
       <c r="H184" s="35"/>
       <c r="I184" s="35"/>
@@ -10387,8 +10387,8 @@
       <c r="B185" s="34"/>
       <c r="C185" s="34"/>
       <c r="D185" s="34"/>
-      <c r="E185" s="92"/>
-      <c r="F185" s="92"/>
+      <c r="E185" s="77"/>
+      <c r="F185" s="77"/>
       <c r="G185" s="1"/>
       <c r="H185" s="35"/>
       <c r="I185" s="35"/>
@@ -10402,8 +10402,8 @@
       <c r="B186" s="34"/>
       <c r="C186" s="34"/>
       <c r="D186" s="34"/>
-      <c r="E186" s="92"/>
-      <c r="F186" s="92"/>
+      <c r="E186" s="77"/>
+      <c r="F186" s="77"/>
       <c r="G186" s="1"/>
       <c r="H186" s="35"/>
       <c r="I186" s="35"/>
@@ -10417,8 +10417,8 @@
       <c r="B187" s="34"/>
       <c r="C187" s="34"/>
       <c r="D187" s="34"/>
-      <c r="E187" s="92"/>
-      <c r="F187" s="92"/>
+      <c r="E187" s="77"/>
+      <c r="F187" s="77"/>
       <c r="G187" s="1"/>
       <c r="H187" s="35"/>
       <c r="I187" s="35"/>
@@ -10432,8 +10432,8 @@
       <c r="B188" s="34"/>
       <c r="C188" s="34"/>
       <c r="D188" s="34"/>
-      <c r="E188" s="92"/>
-      <c r="F188" s="92"/>
+      <c r="E188" s="77"/>
+      <c r="F188" s="77"/>
       <c r="G188" s="1"/>
       <c r="H188" s="35"/>
       <c r="I188" s="35"/>
@@ -10447,8 +10447,8 @@
       <c r="B189" s="34"/>
       <c r="C189" s="34"/>
       <c r="D189" s="34"/>
-      <c r="E189" s="92"/>
-      <c r="F189" s="92"/>
+      <c r="E189" s="77"/>
+      <c r="F189" s="77"/>
       <c r="G189" s="1"/>
       <c r="H189" s="35"/>
       <c r="I189" s="35"/>
@@ -10462,8 +10462,8 @@
       <c r="B190" s="34"/>
       <c r="C190" s="34"/>
       <c r="D190" s="34"/>
-      <c r="E190" s="92"/>
-      <c r="F190" s="92"/>
+      <c r="E190" s="77"/>
+      <c r="F190" s="77"/>
       <c r="G190" s="1"/>
       <c r="H190" s="35"/>
       <c r="I190" s="35"/>
@@ -10477,8 +10477,8 @@
       <c r="B191" s="34"/>
       <c r="C191" s="34"/>
       <c r="D191" s="34"/>
-      <c r="E191" s="92"/>
-      <c r="F191" s="92"/>
+      <c r="E191" s="77"/>
+      <c r="F191" s="77"/>
       <c r="G191" s="1"/>
       <c r="H191" s="35"/>
       <c r="I191" s="35"/>
@@ -10492,8 +10492,8 @@
       <c r="B192" s="34"/>
       <c r="C192" s="34"/>
       <c r="D192" s="34"/>
-      <c r="E192" s="92"/>
-      <c r="F192" s="92"/>
+      <c r="E192" s="77"/>
+      <c r="F192" s="77"/>
       <c r="G192" s="1"/>
       <c r="H192" s="35"/>
       <c r="I192" s="35"/>
@@ -10507,8 +10507,8 @@
       <c r="B193" s="34"/>
       <c r="C193" s="34"/>
       <c r="D193" s="34"/>
-      <c r="E193" s="92"/>
-      <c r="F193" s="92"/>
+      <c r="E193" s="77"/>
+      <c r="F193" s="77"/>
       <c r="G193" s="1"/>
       <c r="H193" s="35"/>
       <c r="I193" s="35"/>
@@ -10522,8 +10522,8 @@
       <c r="B194" s="34"/>
       <c r="C194" s="34"/>
       <c r="D194" s="34"/>
-      <c r="E194" s="92"/>
-      <c r="F194" s="92"/>
+      <c r="E194" s="77"/>
+      <c r="F194" s="77"/>
       <c r="G194" s="1"/>
       <c r="H194" s="35"/>
       <c r="I194" s="35"/>
@@ -10537,8 +10537,8 @@
       <c r="B195" s="34"/>
       <c r="C195" s="34"/>
       <c r="D195" s="34"/>
-      <c r="E195" s="92"/>
-      <c r="F195" s="92"/>
+      <c r="E195" s="77"/>
+      <c r="F195" s="77"/>
       <c r="G195" s="1"/>
       <c r="H195" s="35"/>
       <c r="I195" s="35"/>
@@ -10552,8 +10552,8 @@
       <c r="B196" s="34"/>
       <c r="C196" s="34"/>
       <c r="D196" s="34"/>
-      <c r="E196" s="92"/>
-      <c r="F196" s="92"/>
+      <c r="E196" s="77"/>
+      <c r="F196" s="77"/>
       <c r="G196" s="1"/>
       <c r="H196" s="35"/>
       <c r="I196" s="35"/>
@@ -10567,8 +10567,8 @@
       <c r="B197" s="34"/>
       <c r="C197" s="34"/>
       <c r="D197" s="34"/>
-      <c r="E197" s="92"/>
-      <c r="F197" s="92"/>
+      <c r="E197" s="77"/>
+      <c r="F197" s="77"/>
       <c r="G197" s="1"/>
       <c r="H197" s="35"/>
       <c r="I197" s="35"/>
@@ -10582,8 +10582,8 @@
       <c r="B198" s="34"/>
       <c r="C198" s="34"/>
       <c r="D198" s="34"/>
-      <c r="E198" s="92"/>
-      <c r="F198" s="92"/>
+      <c r="E198" s="77"/>
+      <c r="F198" s="77"/>
       <c r="G198" s="1"/>
       <c r="H198" s="35"/>
       <c r="I198" s="35"/>
@@ -10597,8 +10597,8 @@
       <c r="B199" s="34"/>
       <c r="C199" s="34"/>
       <c r="D199" s="34"/>
-      <c r="E199" s="92"/>
-      <c r="F199" s="92"/>
+      <c r="E199" s="77"/>
+      <c r="F199" s="77"/>
       <c r="G199" s="1"/>
       <c r="H199" s="35"/>
       <c r="I199" s="35"/>
@@ -10612,8 +10612,8 @@
       <c r="B200" s="34"/>
       <c r="C200" s="34"/>
       <c r="D200" s="34"/>
-      <c r="E200" s="92"/>
-      <c r="F200" s="92"/>
+      <c r="E200" s="77"/>
+      <c r="F200" s="77"/>
       <c r="G200" s="1"/>
       <c r="H200" s="35"/>
       <c r="I200" s="35"/>
@@ -10688,32 +10688,32 @@
       <c r="AA1" s="17"/>
     </row>
     <row r="2" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="95"/>
       <c r="F2" s="18"/>
       <c r="G2" s="19"/>
-      <c r="J2" s="69" t="s">
+      <c r="J2" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="71"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="95"/>
       <c r="O2" s="18"/>
       <c r="P2" s="18"/>
       <c r="Q2" s="19"/>
-      <c r="T2" s="69" t="s">
+      <c r="T2" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="71"/>
+      <c r="U2" s="94"/>
+      <c r="V2" s="94"/>
+      <c r="W2" s="94"/>
+      <c r="X2" s="95"/>
       <c r="Y2" s="18"/>
       <c r="Z2" s="18"/>
       <c r="AA2" s="19"/>
@@ -10744,42 +10744,42 @@
       <c r="AA3" s="19"/>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="78"/>
+      <c r="C4" s="92"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="68" t="s">
+      <c r="E4" s="96" t="s">
         <v>58</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="19"/>
-      <c r="J4" s="77" t="s">
+      <c r="J4" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="78"/>
+      <c r="L4" s="92"/>
       <c r="M4" s="18"/>
-      <c r="N4" s="68" t="s">
+      <c r="N4" s="96" t="s">
         <v>58</v>
       </c>
       <c r="O4" s="18"/>
       <c r="P4" s="18"/>
       <c r="Q4" s="19"/>
-      <c r="T4" s="77" t="s">
+      <c r="T4" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="U4" s="78" t="s">
+      <c r="U4" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="V4" s="78"/>
+      <c r="V4" s="92"/>
       <c r="W4" s="18"/>
-      <c r="X4" s="68" t="s">
+      <c r="X4" s="96" t="s">
         <v>58</v>
       </c>
       <c r="Y4" s="18"/>
@@ -10787,27 +10787,27 @@
       <c r="AA4" s="19"/>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="77"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="68"/>
+      <c r="E5" s="96"/>
       <c r="F5" s="10"/>
       <c r="G5" s="21"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
       <c r="M5" s="10"/>
-      <c r="N5" s="68"/>
+      <c r="N5" s="96"/>
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
       <c r="Q5" s="21"/>
       <c r="R5" s="4"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="78"/>
-      <c r="V5" s="78"/>
+      <c r="T5" s="91"/>
+      <c r="U5" s="92"/>
+      <c r="V5" s="92"/>
       <c r="W5" s="18"/>
-      <c r="X5" s="68"/>
+      <c r="X5" s="96"/>
       <c r="Y5" s="18"/>
       <c r="Z5" s="18"/>
       <c r="AA5" s="19"/>
@@ -10841,11 +10841,11 @@
       <c r="A7" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="66" t="e">
+      <c r="B7" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"HúMERO DISTAL")</f>
         <v>#REF!</v>
       </c>
-      <c r="C7" s="67"/>
+      <c r="C7" s="88"/>
       <c r="D7" s="10"/>
       <c r="E7" s="24" t="e">
         <f>(B7/$B$35)</f>
@@ -10856,11 +10856,11 @@
       <c r="J7" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="66" t="e">
+      <c r="K7" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"HUMERO DISTAL")</f>
         <v>#REF!</v>
       </c>
-      <c r="L7" s="67"/>
+      <c r="L7" s="88"/>
       <c r="M7" s="10"/>
       <c r="N7" s="24" t="e">
         <f t="shared" ref="N7:N26" si="0">(K7/$K$35)</f>
@@ -10873,10 +10873,10 @@
       <c r="T7" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="66">
+      <c r="U7" s="87">
         <v>2</v>
       </c>
-      <c r="V7" s="67"/>
+      <c r="V7" s="88"/>
       <c r="W7" s="18"/>
       <c r="X7" s="24" t="e">
         <f t="shared" ref="X7:X26" si="1">U7/$U$35</f>
@@ -10890,11 +10890,11 @@
       <c r="A8" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="66" t="e">
+      <c r="B8" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Peroné")</f>
         <v>#REF!</v>
       </c>
-      <c r="C8" s="67"/>
+      <c r="C8" s="88"/>
       <c r="D8" s="10"/>
       <c r="E8" s="24" t="e">
         <f t="shared" ref="E8:E26" si="2">(B8/$B$35)</f>
@@ -10905,11 +10905,11 @@
       <c r="J8" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="66" t="e">
+      <c r="K8" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"PERONE")</f>
         <v>#REF!</v>
       </c>
-      <c r="L8" s="67"/>
+      <c r="L8" s="88"/>
       <c r="M8" s="10"/>
       <c r="N8" s="24" t="e">
         <f t="shared" si="0"/>
@@ -10922,11 +10922,11 @@
       <c r="T8" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="U8" s="66" t="e">
+      <c r="U8" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"peroné")+1</f>
         <v>#REF!</v>
       </c>
-      <c r="V8" s="67"/>
+      <c r="V8" s="88"/>
       <c r="W8" s="18"/>
       <c r="X8" s="24" t="e">
         <f t="shared" si="1"/>
@@ -10940,11 +10940,11 @@
       <c r="A9" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="66" t="e">
+      <c r="B9" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Tibia DISTAL")</f>
         <v>#REF!</v>
       </c>
-      <c r="C9" s="67"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="10"/>
       <c r="E9" s="24" t="e">
         <f t="shared" si="2"/>
@@ -10955,11 +10955,11 @@
       <c r="J9" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="66" t="e">
+      <c r="K9" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"TIBIA DISTAL")</f>
         <v>#REF!</v>
       </c>
-      <c r="L9" s="67"/>
+      <c r="L9" s="88"/>
       <c r="M9" s="10"/>
       <c r="N9" s="24" t="e">
         <f t="shared" si="0"/>
@@ -10972,11 +10972,11 @@
       <c r="T9" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="U9" s="66" t="e">
+      <c r="U9" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"tibia distal")+2</f>
         <v>#REF!</v>
       </c>
-      <c r="V9" s="67"/>
+      <c r="V9" s="88"/>
       <c r="W9" s="18"/>
       <c r="X9" s="24" t="e">
         <f t="shared" si="1"/>
@@ -10990,11 +10990,11 @@
       <c r="A10" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="66" t="e">
+      <c r="B10" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Húmero proximal")</f>
         <v>#REF!</v>
       </c>
-      <c r="C10" s="67"/>
+      <c r="C10" s="88"/>
       <c r="D10" s="10"/>
       <c r="E10" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11005,11 +11005,11 @@
       <c r="J10" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="66" t="e">
+      <c r="K10" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"HUMERO PROXIMAL")</f>
         <v>#REF!</v>
       </c>
-      <c r="L10" s="67"/>
+      <c r="L10" s="88"/>
       <c r="M10" s="10"/>
       <c r="N10" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11022,11 +11022,11 @@
       <c r="T10" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="U10" s="66" t="e">
+      <c r="U10" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Húmero proximal")</f>
         <v>#REF!</v>
       </c>
-      <c r="V10" s="67"/>
+      <c r="V10" s="88"/>
       <c r="W10" s="18"/>
       <c r="X10" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11040,11 +11040,11 @@
       <c r="A11" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="66" t="e">
+      <c r="B11" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Tibia proximal 4.5")</f>
         <v>#REF!</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="88"/>
       <c r="D11" s="10"/>
       <c r="E11" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11055,11 +11055,11 @@
       <c r="J11" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="K11" s="66" t="e">
+      <c r="K11" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"TIBIA PROXIMAL 4.5")</f>
         <v>#REF!</v>
       </c>
-      <c r="L11" s="67"/>
+      <c r="L11" s="88"/>
       <c r="M11" s="10"/>
       <c r="N11" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11072,11 +11072,11 @@
       <c r="T11" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="U11" s="66" t="e">
+      <c r="U11" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Tibia proximal 4.5")</f>
         <v>#REF!</v>
       </c>
-      <c r="V11" s="67"/>
+      <c r="V11" s="88"/>
       <c r="W11" s="18"/>
       <c r="X11" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11090,11 +11090,11 @@
       <c r="A12" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="66" t="e">
+      <c r="B12" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"DHS")</f>
         <v>#REF!</v>
       </c>
-      <c r="C12" s="67"/>
+      <c r="C12" s="88"/>
       <c r="D12" s="10"/>
       <c r="E12" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11105,11 +11105,11 @@
       <c r="J12" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="K12" s="66" t="e">
+      <c r="K12" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"DHS")</f>
         <v>#REF!</v>
       </c>
-      <c r="L12" s="67"/>
+      <c r="L12" s="88"/>
       <c r="M12" s="10"/>
       <c r="N12" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11122,11 +11122,11 @@
       <c r="T12" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="U12" s="66" t="e">
+      <c r="U12" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"dhs")</f>
         <v>#REF!</v>
       </c>
-      <c r="V12" s="67"/>
+      <c r="V12" s="88"/>
       <c r="W12" s="18"/>
       <c r="X12" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11140,11 +11140,11 @@
       <c r="A13" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="66" t="e">
+      <c r="B13" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"DCS")</f>
         <v>#REF!</v>
       </c>
-      <c r="C13" s="67"/>
+      <c r="C13" s="88"/>
       <c r="D13" s="10"/>
       <c r="E13" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11155,10 +11155,10 @@
       <c r="J13" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="K13" s="66">
+      <c r="K13" s="87">
         <v>0</v>
       </c>
-      <c r="L13" s="67"/>
+      <c r="L13" s="88"/>
       <c r="M13" s="10"/>
       <c r="N13" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11171,11 +11171,11 @@
       <c r="T13" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="U13" s="66" t="e">
+      <c r="U13" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"dcs")</f>
         <v>#REF!</v>
       </c>
-      <c r="V13" s="67"/>
+      <c r="V13" s="88"/>
       <c r="W13" s="18"/>
       <c r="X13" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11189,11 +11189,11 @@
       <c r="A14" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="66" t="e">
+      <c r="B14" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Calcáneo")</f>
         <v>#REF!</v>
       </c>
-      <c r="C14" s="67"/>
+      <c r="C14" s="88"/>
       <c r="D14" s="10"/>
       <c r="E14" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11204,11 +11204,11 @@
       <c r="J14" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="66" t="e">
+      <c r="K14" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"CALCANEO")</f>
         <v>#REF!</v>
       </c>
-      <c r="L14" s="67"/>
+      <c r="L14" s="88"/>
       <c r="M14" s="10"/>
       <c r="N14" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11221,11 +11221,11 @@
       <c r="T14" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="U14" s="66" t="e">
+      <c r="U14" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Calcáneo")</f>
         <v>#REF!</v>
       </c>
-      <c r="V14" s="67"/>
+      <c r="V14" s="88"/>
       <c r="W14" s="18"/>
       <c r="X14" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11239,11 +11239,11 @@
       <c r="A15" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="66" t="e">
+      <c r="B15" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Olecranon")</f>
         <v>#REF!</v>
       </c>
-      <c r="C15" s="67"/>
+      <c r="C15" s="88"/>
       <c r="D15" s="10"/>
       <c r="E15" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11254,11 +11254,11 @@
       <c r="J15" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K15" s="66" t="e">
+      <c r="K15" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"OLECRANON")</f>
         <v>#REF!</v>
       </c>
-      <c r="L15" s="67"/>
+      <c r="L15" s="88"/>
       <c r="M15" s="10"/>
       <c r="N15" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11271,11 +11271,11 @@
       <c r="T15" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="U15" s="66" t="e">
+      <c r="U15" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Olecranon")+1</f>
         <v>#REF!</v>
       </c>
-      <c r="V15" s="67"/>
+      <c r="V15" s="88"/>
       <c r="W15" s="18"/>
       <c r="X15" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11289,11 +11289,11 @@
       <c r="A16" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="66" t="e">
+      <c r="B16" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Fémur distal")</f>
         <v>#REF!</v>
       </c>
-      <c r="C16" s="67"/>
+      <c r="C16" s="88"/>
       <c r="D16" s="10"/>
       <c r="E16" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11304,11 +11304,11 @@
       <c r="J16" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="K16" s="66" t="e">
+      <c r="K16" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"FEMUR DISTAL")</f>
         <v>#REF!</v>
       </c>
-      <c r="L16" s="67"/>
+      <c r="L16" s="88"/>
       <c r="M16" s="10"/>
       <c r="N16" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11321,11 +11321,11 @@
       <c r="T16" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="U16" s="66" t="e">
+      <c r="U16" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Fémur distal")</f>
         <v>#REF!</v>
       </c>
-      <c r="V16" s="67"/>
+      <c r="V16" s="88"/>
       <c r="W16" s="18"/>
       <c r="X16" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11339,11 +11339,11 @@
       <c r="A17" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="66" t="e">
+      <c r="B17" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Minifragmentos")</f>
         <v>#REF!</v>
       </c>
-      <c r="C17" s="67"/>
+      <c r="C17" s="88"/>
       <c r="D17" s="10"/>
       <c r="E17" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11354,11 +11354,11 @@
       <c r="J17" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="66" t="e">
+      <c r="K17" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"MINIFRAGMENTOS")</f>
         <v>#REF!</v>
       </c>
-      <c r="L17" s="67"/>
+      <c r="L17" s="88"/>
       <c r="M17" s="10"/>
       <c r="N17" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11371,11 +11371,11 @@
       <c r="T17" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="U17" s="66" t="e">
+      <c r="U17" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Minifragmentos")</f>
         <v>#REF!</v>
       </c>
-      <c r="V17" s="67"/>
+      <c r="V17" s="88"/>
       <c r="W17" s="18"/>
       <c r="X17" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11389,11 +11389,11 @@
       <c r="A18" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="66" t="e">
+      <c r="B18" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"rectas 3.5")</f>
         <v>#REF!</v>
       </c>
-      <c r="C18" s="67"/>
+      <c r="C18" s="88"/>
       <c r="D18" s="10"/>
       <c r="E18" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11404,11 +11404,11 @@
       <c r="J18" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="K18" s="66" t="e">
+      <c r="K18" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"RECTAS 3.5")+1</f>
         <v>#REF!</v>
       </c>
-      <c r="L18" s="67"/>
+      <c r="L18" s="88"/>
       <c r="M18" s="10"/>
       <c r="N18" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11421,11 +11421,11 @@
       <c r="T18" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="66" t="e">
+      <c r="U18" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"rectas 3.5")</f>
         <v>#REF!</v>
       </c>
-      <c r="V18" s="67"/>
+      <c r="V18" s="88"/>
       <c r="W18" s="18"/>
       <c r="X18" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11439,11 +11439,11 @@
       <c r="A19" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="66" t="e">
+      <c r="B19" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"rectas 4.5")</f>
         <v>#REF!</v>
       </c>
-      <c r="C19" s="67"/>
+      <c r="C19" s="88"/>
       <c r="D19" s="10"/>
       <c r="E19" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11454,11 +11454,11 @@
       <c r="J19" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="K19" s="66" t="e">
+      <c r="K19" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"RECTAS 4.5")</f>
         <v>#REF!</v>
       </c>
-      <c r="L19" s="67"/>
+      <c r="L19" s="88"/>
       <c r="M19" s="10"/>
       <c r="N19" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11471,11 +11471,11 @@
       <c r="T19" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="U19" s="66" t="e">
+      <c r="U19" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"rectas 4.5")+2</f>
         <v>#REF!</v>
       </c>
-      <c r="V19" s="67"/>
+      <c r="V19" s="88"/>
       <c r="W19" s="18"/>
       <c r="X19" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11489,11 +11489,11 @@
       <c r="A20" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="66" t="e">
+      <c r="B20" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"radio DISTAL")</f>
         <v>#REF!</v>
       </c>
-      <c r="C20" s="67"/>
+      <c r="C20" s="88"/>
       <c r="D20" s="10"/>
       <c r="E20" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11504,11 +11504,11 @@
       <c r="J20" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="K20" s="66" t="e">
+      <c r="K20" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"RADIO DISTAL")</f>
         <v>#REF!</v>
       </c>
-      <c r="L20" s="67"/>
+      <c r="L20" s="88"/>
       <c r="M20" s="10"/>
       <c r="N20" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11521,11 +11521,11 @@
       <c r="T20" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="U20" s="66" t="e">
+      <c r="U20" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"radio distal")</f>
         <v>#REF!</v>
       </c>
-      <c r="V20" s="67"/>
+      <c r="V20" s="88"/>
       <c r="W20" s="18"/>
       <c r="X20" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11539,11 +11539,11 @@
       <c r="A21" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="66" t="e">
+      <c r="B21" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"angulo variable")</f>
         <v>#REF!</v>
       </c>
-      <c r="C21" s="67"/>
+      <c r="C21" s="88"/>
       <c r="D21" s="10"/>
       <c r="E21" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11554,11 +11554,11 @@
       <c r="J21" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="K21" s="66" t="e">
+      <c r="K21" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"ANGULO VARIABLE")</f>
         <v>#REF!</v>
       </c>
-      <c r="L21" s="67"/>
+      <c r="L21" s="88"/>
       <c r="M21" s="10"/>
       <c r="N21" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11571,11 +11571,11 @@
       <c r="T21" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="U21" s="66" t="e">
+      <c r="U21" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"angulo variable")</f>
         <v>#REF!</v>
       </c>
-      <c r="V21" s="67"/>
+      <c r="V21" s="88"/>
       <c r="W21" s="18"/>
       <c r="X21" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11589,11 +11589,11 @@
       <c r="A22" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="66" t="e">
+      <c r="B22" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"clavicular")</f>
         <v>#REF!</v>
       </c>
-      <c r="C22" s="67"/>
+      <c r="C22" s="88"/>
       <c r="D22" s="10"/>
       <c r="E22" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11604,11 +11604,11 @@
       <c r="J22" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="K22" s="66" t="e">
+      <c r="K22" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"CLAVICULA")</f>
         <v>#REF!</v>
       </c>
-      <c r="L22" s="67"/>
+      <c r="L22" s="88"/>
       <c r="M22" s="10"/>
       <c r="N22" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11621,11 +11621,11 @@
       <c r="T22" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="U22" s="66" t="e">
+      <c r="U22" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"clavicular")</f>
         <v>#REF!</v>
       </c>
-      <c r="V22" s="67"/>
+      <c r="V22" s="88"/>
       <c r="W22" s="18"/>
       <c r="X22" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11639,11 +11639,11 @@
       <c r="A23" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="66" t="e">
+      <c r="B23" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"reconstrucción")</f>
         <v>#REF!</v>
       </c>
-      <c r="C23" s="67"/>
+      <c r="C23" s="88"/>
       <c r="D23" s="10"/>
       <c r="E23" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11654,11 +11654,11 @@
       <c r="J23" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="K23" s="66" t="e">
+      <c r="K23" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"RECONSTRUCCION")</f>
         <v>#REF!</v>
       </c>
-      <c r="L23" s="67"/>
+      <c r="L23" s="88"/>
       <c r="M23" s="10"/>
       <c r="N23" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11671,11 +11671,11 @@
       <c r="T23" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="U23" s="66" t="e">
+      <c r="U23" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"reconstrucción")</f>
         <v>#REF!</v>
       </c>
-      <c r="V23" s="67"/>
+      <c r="V23" s="88"/>
       <c r="W23" s="18"/>
       <c r="X23" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11689,11 +11689,11 @@
       <c r="A24" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="66" t="e">
+      <c r="B24" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Tibia proximal 3.5")</f>
         <v>#REF!</v>
       </c>
-      <c r="C24" s="67"/>
+      <c r="C24" s="88"/>
       <c r="D24" s="10"/>
       <c r="E24" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11704,10 +11704,10 @@
       <c r="J24" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="K24" s="66">
+      <c r="K24" s="87">
         <v>0</v>
       </c>
-      <c r="L24" s="67"/>
+      <c r="L24" s="88"/>
       <c r="M24" s="10"/>
       <c r="N24" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11720,11 +11720,11 @@
       <c r="T24" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="U24" s="66" t="e">
+      <c r="U24" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"tibia proximal 3.5")</f>
         <v>#REF!</v>
       </c>
-      <c r="V24" s="67"/>
+      <c r="V24" s="88"/>
       <c r="W24" s="18"/>
       <c r="X24" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11738,11 +11738,11 @@
       <c r="A25" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="66" t="e">
+      <c r="B25" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Tercio de caña")</f>
         <v>#REF!</v>
       </c>
-      <c r="C25" s="67"/>
+      <c r="C25" s="88"/>
       <c r="D25" s="10"/>
       <c r="E25" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11753,10 +11753,10 @@
       <c r="J25" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="K25" s="66">
+      <c r="K25" s="87">
         <v>1</v>
       </c>
-      <c r="L25" s="67"/>
+      <c r="L25" s="88"/>
       <c r="M25" s="10"/>
       <c r="N25" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11769,11 +11769,11 @@
       <c r="T25" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="U25" s="66" t="e">
+      <c r="U25" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"tercio de caña")</f>
         <v>#REF!</v>
       </c>
-      <c r="V25" s="67"/>
+      <c r="V25" s="88"/>
       <c r="W25" s="18"/>
       <c r="X25" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11787,11 +11787,11 @@
       <c r="A26" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="66" t="e">
+      <c r="B26" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Fémur proximal")</f>
         <v>#REF!</v>
       </c>
-      <c r="C26" s="67"/>
+      <c r="C26" s="88"/>
       <c r="D26" s="10"/>
       <c r="E26" s="24" t="e">
         <f t="shared" si="2"/>
@@ -11802,10 +11802,10 @@
       <c r="J26" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="K26" s="66">
+      <c r="K26" s="87">
         <v>0</v>
       </c>
-      <c r="L26" s="67"/>
+      <c r="L26" s="88"/>
       <c r="M26" s="10"/>
       <c r="N26" s="24" t="e">
         <f t="shared" si="0"/>
@@ -11818,10 +11818,10 @@
       <c r="T26" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="U26" s="66">
+      <c r="U26" s="87">
         <v>0</v>
       </c>
-      <c r="V26" s="67"/>
+      <c r="V26" s="88"/>
       <c r="W26" s="18"/>
       <c r="X26" s="24" t="e">
         <f t="shared" si="1"/>
@@ -11860,11 +11860,11 @@
       <c r="A28" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="66" t="e">
+      <c r="B28" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"no")</f>
         <v>#REF!</v>
       </c>
-      <c r="C28" s="67"/>
+      <c r="C28" s="88"/>
       <c r="D28" s="10"/>
       <c r="E28" s="24" t="e">
         <f>B28/B35</f>
@@ -11875,11 +11875,11 @@
       <c r="J28" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="K28" s="66" t="e">
+      <c r="K28" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"NO")</f>
         <v>#REF!</v>
       </c>
-      <c r="L28" s="67"/>
+      <c r="L28" s="88"/>
       <c r="M28" s="10"/>
       <c r="N28" s="24" t="e">
         <f>K28/K35</f>
@@ -11892,11 +11892,11 @@
       <c r="T28" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="U28" s="66" t="e">
+      <c r="U28" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"no")</f>
         <v>#REF!</v>
       </c>
-      <c r="V28" s="67"/>
+      <c r="V28" s="88"/>
       <c r="W28" s="18"/>
       <c r="X28" s="24" t="e">
         <f>U28/U35</f>
@@ -11935,11 +11935,11 @@
       <c r="A30" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="66" t="e">
+      <c r="B30" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"ret")</f>
         <v>#REF!</v>
       </c>
-      <c r="C30" s="67"/>
+      <c r="C30" s="88"/>
       <c r="D30" s="10"/>
       <c r="E30" s="24" t="e">
         <f>B30/B35</f>
@@ -11950,10 +11950,10 @@
       <c r="J30" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="K30" s="66">
+      <c r="K30" s="87">
         <v>3</v>
       </c>
-      <c r="L30" s="67"/>
+      <c r="L30" s="88"/>
       <c r="M30" s="10"/>
       <c r="N30" s="24" t="e">
         <f>K30/K35</f>
@@ -11966,10 +11966,10 @@
       <c r="T30" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="U30" s="66">
+      <c r="U30" s="87">
         <v>1</v>
       </c>
-      <c r="V30" s="67"/>
+      <c r="V30" s="88"/>
       <c r="W30" s="18"/>
       <c r="X30" s="24" t="e">
         <f>U30/U35</f>
@@ -12008,11 +12008,11 @@
       <c r="A32" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="66" t="e">
+      <c r="B32" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"agujas")</f>
         <v>#REF!</v>
       </c>
-      <c r="C32" s="67"/>
+      <c r="C32" s="88"/>
       <c r="D32" s="10"/>
       <c r="E32" s="24" t="e">
         <f>(B32/B35)</f>
@@ -12023,11 +12023,11 @@
       <c r="J32" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="K32" s="66" t="e">
+      <c r="K32" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"AGUJAS")</f>
         <v>#REF!</v>
       </c>
-      <c r="L32" s="67"/>
+      <c r="L32" s="88"/>
       <c r="M32" s="10"/>
       <c r="N32" s="24" t="e">
         <f>(K32/K35)</f>
@@ -12039,11 +12039,11 @@
       <c r="T32" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="U32" s="66" t="e">
+      <c r="U32" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"agujas")</f>
         <v>#REF!</v>
       </c>
-      <c r="V32" s="67"/>
+      <c r="V32" s="88"/>
       <c r="W32" s="10"/>
       <c r="X32" s="24" t="e">
         <f>(U32/U35)</f>
@@ -12107,56 +12107,56 @@
       <c r="A35" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="67" t="e">
+      <c r="B35" s="88" t="e">
         <f>SUM(B7:C26)</f>
         <v>#REF!</v>
       </c>
-      <c r="C35" s="67"/>
+      <c r="C35" s="88"/>
       <c r="D35" s="10"/>
       <c r="E35" s="33" t="e">
         <f>B35/26</f>
         <v>#REF!</v>
       </c>
-      <c r="F35" s="74" t="s">
+      <c r="F35" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="G35" s="79"/>
+      <c r="G35" s="90"/>
       <c r="J35" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="K35" s="67" t="e">
+      <c r="K35" s="88" t="e">
         <f>SUM(K7:L26)</f>
         <v>#REF!</v>
       </c>
-      <c r="L35" s="67"/>
+      <c r="L35" s="88"/>
       <c r="M35" s="10"/>
       <c r="N35" s="33" t="e">
         <f>K35/26</f>
         <v>#REF!</v>
       </c>
-      <c r="O35" s="74" t="s">
+      <c r="O35" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="P35" s="74"/>
+      <c r="P35" s="89"/>
       <c r="Q35" s="32"/>
       <c r="R35" s="5"/>
       <c r="T35" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="U35" s="67" t="e">
+      <c r="U35" s="88" t="e">
         <f>SUM(U7:V26)</f>
         <v>#REF!</v>
       </c>
-      <c r="V35" s="67"/>
+      <c r="V35" s="88"/>
       <c r="W35" s="10"/>
       <c r="X35" s="33" t="e">
         <f>U35/27</f>
         <v>#REF!</v>
       </c>
-      <c r="Y35" s="74" t="s">
+      <c r="Y35" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="Z35" s="74"/>
+      <c r="Z35" s="89"/>
       <c r="AA35" s="19"/>
     </row>
     <row r="36" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12198,13 +12198,13 @@
     </row>
     <row r="40" spans="1:35" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I40" s="22"/>
-      <c r="J40" s="69" t="s">
+      <c r="J40" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="K40" s="70"/>
-      <c r="L40" s="70"/>
-      <c r="M40" s="70"/>
-      <c r="N40" s="71"/>
+      <c r="K40" s="94"/>
+      <c r="L40" s="94"/>
+      <c r="M40" s="94"/>
+      <c r="N40" s="95"/>
       <c r="O40" s="18"/>
       <c r="P40" s="18"/>
       <c r="Q40" s="19"/>
@@ -12226,7 +12226,7 @@
       <c r="K42" s="18"/>
       <c r="L42" s="18"/>
       <c r="M42" s="18"/>
-      <c r="N42" s="68" t="s">
+      <c r="N42" s="96" t="s">
         <v>58</v>
       </c>
       <c r="O42" s="18"/>
@@ -12238,12 +12238,12 @@
       <c r="J43" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="K43" s="67" t="s">
+      <c r="K43" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="L43" s="67"/>
+      <c r="L43" s="88"/>
       <c r="M43" s="10"/>
-      <c r="N43" s="68"/>
+      <c r="N43" s="96"/>
       <c r="O43" s="18"/>
       <c r="P43" s="18"/>
       <c r="Q43" s="19"/>
@@ -12264,18 +12264,18 @@
       <c r="P44" s="18"/>
       <c r="Q44" s="19"/>
       <c r="X44" s="12"/>
-      <c r="Y44" s="72"/>
-      <c r="Z44" s="72"/>
+      <c r="Y44" s="99"/>
+      <c r="Z44" s="99"/>
       <c r="AA44" s="13"/>
       <c r="AB44" s="14"/>
       <c r="AE44" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="AF44" s="66">
+      <c r="AF44" s="87">
         <f>SUM(AF17:AG36)</f>
         <v>0</v>
       </c>
-      <c r="AG44" s="73"/>
+      <c r="AG44" s="100"/>
       <c r="AI44" s="9">
         <f>SUM(AI17:AI36)</f>
         <v>0</v>
@@ -12297,11 +12297,11 @@
       <c r="J46" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K46" s="75" t="e">
+      <c r="K46" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Húmero distal")+1</f>
         <v>#REF!</v>
       </c>
-      <c r="L46" s="76"/>
+      <c r="L46" s="98"/>
       <c r="M46" s="18"/>
       <c r="N46" s="24" t="e">
         <f>K46/$K$75</f>
@@ -12316,11 +12316,11 @@
       <c r="J47" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K47" s="75" t="e">
+      <c r="K47" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Peroné")</f>
         <v>#REF!</v>
       </c>
-      <c r="L47" s="76"/>
+      <c r="L47" s="98"/>
       <c r="M47" s="18"/>
       <c r="N47" s="24" t="e">
         <f t="shared" ref="N47:N65" si="3">K47/$K$75</f>
@@ -12335,11 +12335,11 @@
       <c r="J48" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K48" s="75" t="e">
+      <c r="K48" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Tibia distal")+2</f>
         <v>#REF!</v>
       </c>
-      <c r="L48" s="76"/>
+      <c r="L48" s="98"/>
       <c r="M48" s="18"/>
       <c r="N48" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12350,18 +12350,18 @@
       <c r="Q48" s="19"/>
     </row>
     <row r="49" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B49" s="65"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="65"/>
+      <c r="B49" s="101"/>
+      <c r="C49" s="101"/>
+      <c r="D49" s="101"/>
       <c r="I49" s="22"/>
       <c r="J49" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="K49" s="75" t="e">
+      <c r="K49" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Húmero proximal")</f>
         <v>#REF!</v>
       </c>
-      <c r="L49" s="76"/>
+      <c r="L49" s="98"/>
       <c r="M49" s="18"/>
       <c r="N49" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12376,11 +12376,11 @@
       <c r="J50" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K50" s="75" t="e">
+      <c r="K50" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Tibia proximal 4.5")</f>
         <v>#REF!</v>
       </c>
-      <c r="L50" s="76"/>
+      <c r="L50" s="98"/>
       <c r="M50" s="18"/>
       <c r="N50" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12395,11 +12395,11 @@
       <c r="J51" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K51" s="75" t="e">
+      <c r="K51" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"DHS")</f>
         <v>#REF!</v>
       </c>
-      <c r="L51" s="76"/>
+      <c r="L51" s="98"/>
       <c r="M51" s="18"/>
       <c r="N51" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12414,11 +12414,11 @@
       <c r="J52" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K52" s="75" t="e">
+      <c r="K52" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"DCS")</f>
         <v>#REF!</v>
       </c>
-      <c r="L52" s="76"/>
+      <c r="L52" s="98"/>
       <c r="M52" s="18"/>
       <c r="N52" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12433,11 +12433,11 @@
       <c r="J53" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K53" s="75" t="e">
+      <c r="K53" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Calcáneo")</f>
         <v>#REF!</v>
       </c>
-      <c r="L53" s="76"/>
+      <c r="L53" s="98"/>
       <c r="M53" s="18"/>
       <c r="N53" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12452,11 +12452,11 @@
       <c r="J54" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="K54" s="75" t="e">
+      <c r="K54" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Olecranon")</f>
         <v>#REF!</v>
       </c>
-      <c r="L54" s="76"/>
+      <c r="L54" s="98"/>
       <c r="M54" s="18"/>
       <c r="N54" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12471,11 +12471,11 @@
       <c r="J55" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K55" s="75" t="e">
+      <c r="K55" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Fémur distal")</f>
         <v>#REF!</v>
       </c>
-      <c r="L55" s="76"/>
+      <c r="L55" s="98"/>
       <c r="M55" s="18"/>
       <c r="N55" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12490,11 +12490,11 @@
       <c r="J56" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="K56" s="75" t="e">
+      <c r="K56" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Minifragmentos")+1</f>
         <v>#REF!</v>
       </c>
-      <c r="L56" s="76"/>
+      <c r="L56" s="98"/>
       <c r="M56" s="18"/>
       <c r="N56" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12509,11 +12509,11 @@
       <c r="J57" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="K57" s="75" t="e">
+      <c r="K57" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"rectas 3.5")+1</f>
         <v>#REF!</v>
       </c>
-      <c r="L57" s="76"/>
+      <c r="L57" s="98"/>
       <c r="M57" s="18"/>
       <c r="N57" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12528,11 +12528,11 @@
       <c r="J58" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="K58" s="75" t="e">
+      <c r="K58" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Rectas 4.5")+2</f>
         <v>#REF!</v>
       </c>
-      <c r="L58" s="76"/>
+      <c r="L58" s="98"/>
       <c r="M58" s="18"/>
       <c r="N58" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12547,11 +12547,11 @@
       <c r="J59" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="K59" s="75" t="e">
+      <c r="K59" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Radio distal")</f>
         <v>#REF!</v>
       </c>
-      <c r="L59" s="76"/>
+      <c r="L59" s="98"/>
       <c r="M59" s="18"/>
       <c r="N59" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12566,11 +12566,11 @@
       <c r="J60" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="K60" s="75" t="e">
+      <c r="K60" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Angulo variable")</f>
         <v>#REF!</v>
       </c>
-      <c r="L60" s="76"/>
+      <c r="L60" s="98"/>
       <c r="M60" s="18"/>
       <c r="N60" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12585,11 +12585,11 @@
       <c r="J61" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="K61" s="75" t="e">
+      <c r="K61" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Clavicular")+1</f>
         <v>#REF!</v>
       </c>
-      <c r="L61" s="76"/>
+      <c r="L61" s="98"/>
       <c r="M61" s="18"/>
       <c r="N61" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12604,11 +12604,11 @@
       <c r="J62" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="K62" s="75" t="e">
+      <c r="K62" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Reconstrucción")+3</f>
         <v>#REF!</v>
       </c>
-      <c r="L62" s="76"/>
+      <c r="L62" s="98"/>
       <c r="M62" s="18"/>
       <c r="N62" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12623,11 +12623,11 @@
       <c r="J63" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="K63" s="75" t="e">
+      <c r="K63" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Tibia proximal 3.5")</f>
         <v>#REF!</v>
       </c>
-      <c r="L63" s="76"/>
+      <c r="L63" s="98"/>
       <c r="M63" s="18"/>
       <c r="N63" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12642,11 +12642,11 @@
       <c r="J64" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="K64" s="75" t="e">
+      <c r="K64" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Tercio de caña")+2</f>
         <v>#REF!</v>
       </c>
-      <c r="L64" s="76"/>
+      <c r="L64" s="98"/>
       <c r="M64" s="18"/>
       <c r="N64" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12661,11 +12661,11 @@
       <c r="J65" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K65" s="75" t="e">
+      <c r="K65" s="97" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"Fémur proximal")</f>
         <v>#REF!</v>
       </c>
-      <c r="L65" s="76"/>
+      <c r="L65" s="98"/>
       <c r="M65" s="18"/>
       <c r="N65" s="24" t="e">
         <f t="shared" si="3"/>
@@ -12702,11 +12702,11 @@
       <c r="J68" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K68" s="66" t="e">
+      <c r="K68" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"no")</f>
         <v>#REF!</v>
       </c>
-      <c r="L68" s="67"/>
+      <c r="L68" s="88"/>
       <c r="M68" s="18"/>
       <c r="N68" s="24" t="e">
         <f>K68/K75</f>
@@ -12732,11 +12732,11 @@
       <c r="J70" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K70" s="66" t="e">
+      <c r="K70" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"ret")</f>
         <v>#REF!</v>
       </c>
-      <c r="L70" s="67"/>
+      <c r="L70" s="88"/>
       <c r="M70" s="18"/>
       <c r="N70" s="24" t="e">
         <f>K70/K75</f>
@@ -12762,11 +12762,11 @@
       <c r="J72" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K72" s="66" t="e">
+      <c r="K72" s="87" t="e">
         <f>COUNTIF('Control de cirugía'!#REF!,"agujas")</f>
         <v>#REF!</v>
       </c>
-      <c r="L72" s="67"/>
+      <c r="L72" s="88"/>
       <c r="M72" s="18"/>
       <c r="N72" s="24" t="e">
         <f>K72/K75</f>
@@ -12803,20 +12803,20 @@
       <c r="J75" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K75" s="67" t="e">
+      <c r="K75" s="88" t="e">
         <f>SUM(K46:L65)</f>
         <v>#REF!</v>
       </c>
-      <c r="L75" s="67"/>
+      <c r="L75" s="88"/>
       <c r="M75" s="18"/>
       <c r="N75" s="33" t="e">
         <f>K75/27</f>
         <v>#REF!</v>
       </c>
-      <c r="O75" s="74" t="s">
+      <c r="O75" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="P75" s="74"/>
+      <c r="P75" s="89"/>
       <c r="Q75" s="19"/>
     </row>
     <row r="76" spans="9:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12832,28 +12832,78 @@
     </row>
   </sheetData>
   <mergeCells count="118">
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="X4:X5"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="U28:V28"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="Y44:Z44"/>
+    <mergeCell ref="AF44:AG44"/>
+    <mergeCell ref="Y35:Z35"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="K61:L61"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="K60:L60"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="K53:L53"/>
     <mergeCell ref="O75:P75"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:L5"/>
@@ -12878,78 +12928,28 @@
     <mergeCell ref="J2:N2"/>
     <mergeCell ref="U32:V32"/>
     <mergeCell ref="K9:L9"/>
-    <mergeCell ref="Y44:Z44"/>
-    <mergeCell ref="AF44:AG44"/>
-    <mergeCell ref="Y35:Z35"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="K65:L65"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="K61:L61"/>
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="K63:L63"/>
-    <mergeCell ref="K64:L64"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="K60:L60"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="K52:L52"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="X4:X5"/>
-    <mergeCell ref="T2:X2"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>